<commit_message>
add automatic generation of opcode.h
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="277">
   <si>
     <t>Name</t>
   </si>
@@ -67,9 +67,6 @@
     <t>NOR</t>
   </si>
   <si>
-    <t>Cat</t>
-  </si>
-  <si>
     <t>Basic</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>RETN</t>
   </si>
   <si>
-    <t>SP -= sizeof(PC), PC = RAM[SP]</t>
-  </si>
-  <si>
     <t>Will swap to const mode in instructions</t>
   </si>
   <si>
@@ -256,9 +250,6 @@
     <t>SHL</t>
   </si>
   <si>
-    <t>AHSR</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -424,9 +415,6 @@
     <t>SHL32</t>
   </si>
   <si>
-    <t>AHSR32</t>
-  </si>
-  <si>
     <t>MULU</t>
   </si>
   <si>
@@ -452,15 +440,6 @@
   </si>
   <si>
     <t>DIVF</t>
-  </si>
-  <si>
-    <t>See 32-bit notes</t>
-  </si>
-  <si>
-    <t>! 32-bit notes !</t>
-  </si>
-  <si>
-    <t>Works only on R1 and R3 (will then also use R2/R4) Consts will, when used, be 32 bits (bit 8-31)!</t>
   </si>
   <si>
     <r>
@@ -903,6 +882,18 @@
   </si>
   <si>
     <t>RAM[IHBASE+Reg*2] = Reg2 (0 for disable)</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>SP -= 2, PC = RAM[SP]</t>
+  </si>
+  <si>
+    <t>ASHR</t>
+  </si>
+  <si>
+    <t>ASHR32</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1006,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1078,13 +1069,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1097,6 +1081,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1416,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,33 +1421,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>273</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1472,24 +1460,22 @@
         <v>00</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C3" s="2">
         <f>C2+1</f>
@@ -1500,21 +1486,21 @@
         <v>01</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="22">
         <f>C3+1</f>
@@ -1525,18 +1511,18 @@
         <v>02</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
         <v>251</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:C72" si="1">C4+1</f>
@@ -1547,21 +1533,19 @@
         <v>03</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="1"/>
@@ -1572,21 +1556,19 @@
         <v>04</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>259</v>
-      </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
@@ -1597,18 +1579,18 @@
         <v>05</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
@@ -1619,12 +1601,12 @@
         <v>06</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -1638,16 +1620,16 @@
         <v>07</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1663,16 +1645,16 @@
         <v>08</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1688,16 +1670,16 @@
         <v>09</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1713,16 +1695,16 @@
         <v>0A</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1738,21 +1720,21 @@
         <v>0B</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="1"/>
@@ -1763,21 +1745,21 @@
         <v>0C</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
@@ -1788,21 +1770,21 @@
         <v>0D</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>75</v>
+        <v>275</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="1"/>
@@ -1813,21 +1795,21 @@
         <v>0E</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
@@ -1838,21 +1820,21 @@
         <v>0F</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
@@ -1863,21 +1845,21 @@
         <v>10</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -1891,16 +1873,16 @@
         <v>11</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1916,16 +1898,16 @@
         <v>12</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1941,16 +1923,16 @@
         <v>13</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1967,16 +1949,16 @@
         <v>14</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1995,16 +1977,16 @@
         <v>15</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2012,7 +1994,7 @@
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="1"/>
@@ -2023,26 +2005,26 @@
         <v>16</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C25" s="22">
         <f t="shared" si="1"/>
@@ -2053,21 +2035,21 @@
         <v>17</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C26" s="22">
         <f t="shared" si="1"/>
@@ -2078,21 +2060,19 @@
         <v>18</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>141</v>
-      </c>
+      <c r="A27" s="29"/>
       <c r="B27" s="22" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C27" s="22">
         <f t="shared" si="1"/>
@@ -2103,22 +2083,22 @@
         <v>19</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30"/>
       <c r="B28" s="22" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C28" s="22">
         <f t="shared" si="1"/>
@@ -2129,18 +2109,18 @@
         <v>1A</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="22" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C29" s="22">
         <f t="shared" si="1"/>
@@ -2151,24 +2131,24 @@
         <v>1B</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="22">
         <f t="shared" si="1"/>
@@ -2179,21 +2159,21 @@
         <v>1C</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="1"/>
@@ -2204,10 +2184,10 @@
         <v>1D</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -2217,7 +2197,7 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="1"/>
@@ -2228,10 +2208,10 @@
         <v>1E</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2241,7 +2221,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="2">
         <f t="shared" si="1"/>
@@ -2252,10 +2232,10 @@
         <v>1F</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -2265,7 +2245,7 @@
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="1"/>
@@ -2276,10 +2256,10 @@
         <v>20</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2288,7 +2268,7 @@
     </row>
     <row r="35" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="22" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C35" s="22">
         <f t="shared" si="1"/>
@@ -2299,17 +2279,17 @@
         <v>21</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C36" s="22">
         <f t="shared" si="1"/>
@@ -2320,10 +2300,10 @@
         <v>22</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2333,7 +2313,7 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="2">
         <f t="shared" si="1"/>
@@ -2344,16 +2324,16 @@
         <v>23</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -2361,27 +2341,27 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="D38" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="2">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="D38" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G38" s="22" t="s">
-        <v>35</v>
-      </c>
       <c r="H38" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -2389,7 +2369,7 @@
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="2">
         <f t="shared" si="1"/>
@@ -2400,23 +2380,23 @@
         <v>25</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J39" s="37" t="s">
-        <v>144</v>
+        <v>37</v>
+      </c>
+      <c r="J39" s="34" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C40" s="2">
         <f t="shared" si="1"/>
@@ -2427,20 +2407,20 @@
         <v>26</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="37"/>
+      <c r="J40" s="34"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C41" s="2">
         <f t="shared" si="1"/>
@@ -2451,68 +2431,68 @@
         <v>27</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="37"/>
+      <c r="J41" s="34"/>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="C42" s="2">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
       <c r="D42" s="19" t="str">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F42" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="37"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="C43" s="2">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
       <c r="D43" s="19" t="str">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="37"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C44" s="2">
         <f t="shared" si="1"/>
@@ -2523,20 +2503,20 @@
         <v>2A</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="37"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C45" s="2">
         <f t="shared" si="1"/>
@@ -2547,20 +2527,20 @@
         <v>2B</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="37"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" s="2">
         <f t="shared" si="1"/>
@@ -2571,24 +2551,24 @@
         <v>2C</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="I46" s="2"/>
-      <c r="J46" s="37"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" s="2">
         <f t="shared" si="1"/>
@@ -2599,24 +2579,24 @@
         <v>2D</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="I47" s="2"/>
-      <c r="J47" s="37"/>
+      <c r="J47" s="34"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" si="1"/>
@@ -2627,23 +2607,23 @@
         <v>2E</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
-        <v>45</v>
+        <v>274</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="C49" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2653,14 +2633,14 @@
         <v>2F</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F49" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="2" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -2668,7 +2648,7 @@
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C50" s="2">
         <f t="shared" si="1"/>
@@ -2679,16 +2659,16 @@
         <v>30</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G50" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2696,7 +2676,7 @@
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C51" s="2">
         <f t="shared" si="1"/>
@@ -2707,12 +2687,12 @@
         <v>31</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2720,7 +2700,7 @@
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C52" s="2">
         <f t="shared" si="1"/>
@@ -2731,12 +2711,12 @@
         <v>32</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2744,7 +2724,7 @@
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C53" s="2">
         <f t="shared" si="1"/>
@@ -2755,19 +2735,19 @@
         <v>33</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
     <row r="54" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C54" s="15">
         <f t="shared" si="1"/>
@@ -2778,15 +2758,15 @@
         <v>34</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="15" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C55" s="15">
         <f t="shared" si="1"/>
@@ -2797,15 +2777,15 @@
         <v>35</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="17" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C56" s="17">
         <f t="shared" si="1"/>
@@ -2816,15 +2796,15 @@
         <v>36</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="17" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C57" s="17">
         <f t="shared" si="1"/>
@@ -2835,15 +2815,15 @@
         <v>37</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="22" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C58" s="22">
         <f t="shared" si="1"/>
@@ -2854,282 +2834,280 @@
         <v>38</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="H58" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="22">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="D59" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="2">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="D60" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3A</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="12"/>
+      <c r="B61" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C61" s="2">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="D61" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3B</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="22">
-        <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
-      <c r="D59" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59" s="2" t="s">
+      <c r="C62" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="D62" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3C</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="G62" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="2">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="D63" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3D</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="2">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="D64" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3E</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="12"/>
+      <c r="B65" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" s="2">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="D65" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3F</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C66" s="2">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="D66" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" s="5" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" s="2">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-      <c r="D60" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>3A</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G60" s="2" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
+      <c r="B67" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" s="2">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="D67" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="G67" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" s="5" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="34"/>
-      <c r="B61" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C61" s="2">
-        <f t="shared" si="1"/>
-        <v>59</v>
-      </c>
-      <c r="D61" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>3B</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G61" s="2" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="12"/>
+      <c r="B68" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="2">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="D68" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="G68" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H68" s="5" t="s">
         <v>262</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
-      <c r="B62" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" s="2">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="D62" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>3C</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="34"/>
-      <c r="B63" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" s="2">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="D63" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>3D</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="34"/>
-      <c r="B64" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" s="2">
-        <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-      <c r="D64" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>3E</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
-      <c r="B65" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C65" s="2">
-        <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="D65" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>3F</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="34"/>
-      <c r="B66" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C66" s="2">
-        <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="D66" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="34"/>
-      <c r="B67" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="2">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="D67" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="E67" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H67" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="34"/>
-      <c r="B68" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C68" s="2">
-        <f t="shared" si="1"/>
-        <v>66</v>
-      </c>
-      <c r="D68" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C69" s="2">
         <f t="shared" si="1"/>
@@ -3140,50 +3118,48 @@
         <v>43</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G69" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="12"/>
+      <c r="B70" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="D70" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H69" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="B70" t="s">
-        <v>138</v>
-      </c>
-      <c r="C70" s="2">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="D70" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="G70" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
+      <c r="A71" s="12"/>
       <c r="B71" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C71" s="2">
         <f t="shared" si="1"/>
@@ -3194,22 +3170,22 @@
         <v>45</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
+      <c r="A72" s="12"/>
       <c r="B72" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C72" s="2">
         <f t="shared" si="1"/>
@@ -3220,44 +3196,41 @@
         <v>46</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
+      <c r="E73" s="10"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
+      <c r="A74" s="39"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="39"/>
+      <c r="H74" s="39"/>
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="35"/>
+      <c r="A75" s="38"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="38"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
@@ -3272,11 +3245,7 @@
       <c r="A79" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A60:A68"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A75:H75"/>
-    <mergeCell ref="A74:H74"/>
+  <mergeCells count="1">
     <mergeCell ref="J39:J47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3302,13 +3271,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3316,13 +3285,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3331,13 +3300,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3346,13 +3315,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3361,13 +3330,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3376,13 +3345,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3391,13 +3360,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3406,13 +3375,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3421,18 +3390,18 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3440,13 +3409,13 @@
         <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3455,13 +3424,13 @@
         <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3470,13 +3439,13 @@
         <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
@@ -3510,28 +3479,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3539,17 +3508,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
       <c r="E2" s="25"/>
       <c r="F2" s="23" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G2" s="23"/>
       <c r="I2" s="26" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3558,7 +3527,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="23"/>
@@ -3566,7 +3535,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="I3" s="27" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3575,7 +3544,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="23"/>
@@ -3583,7 +3552,7 @@
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
       <c r="I4" s="28" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3592,18 +3561,18 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="23" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="23" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3612,13 +3581,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="23" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G6" s="23"/>
     </row>
@@ -3645,7 +3614,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3657,13 +3626,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>111</v>
+        <v>22</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3672,10 +3641,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
+        <v>23</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3683,12 +3652,12 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="D4" s="39"/>
+        <v>24</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="36"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3696,10 +3665,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
+        <v>25</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3707,10 +3676,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3719,10 +3688,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3731,13 +3700,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>202</v>
+        <v>143</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>195</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3746,9 +3715,9 @@
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9" s="38"/>
+        <v>144</v>
+      </c>
+      <c r="C9" s="35"/>
       <c r="D9" s="31"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3757,10 +3726,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D10" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3769,10 +3738,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3799,10 +3768,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3811,10 +3780,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D16" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3823,10 +3792,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3848,8 +3817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3862,16 +3831,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3879,12 +3848,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" s="38"/>
+        <v>153</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="35"/>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -3892,10 +3861,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+        <v>154</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
     </row>
     <row r="4" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
@@ -3903,10 +3872,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+        <v>158</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
@@ -3914,12 +3883,12 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="38"/>
+        <v>231</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="35"/>
       <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3928,10 +3897,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
+        <v>232</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3940,10 +3909,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+        <v>233</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3952,10 +3921,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+        <v>234</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="22"/>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3964,10 +3933,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+        <v>235</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3976,12 +3945,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="38"/>
+        <v>110</v>
+      </c>
+      <c r="D10" s="35"/>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -3989,12 +3958,12 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="38"/>
+        <v>88</v>
+      </c>
+      <c r="D11" s="35"/>
     </row>
     <row r="12" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
@@ -4002,12 +3971,12 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="38"/>
+        <v>84</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
@@ -4015,10 +3984,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+        <v>105</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
@@ -4026,10 +3995,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+        <v>106</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
@@ -4037,10 +4006,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+        <v>107</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
@@ -4048,12 +4017,12 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="38"/>
+        <v>75</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
@@ -4061,10 +4030,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="38"/>
+        <v>148</v>
+      </c>
+      <c r="C17" s="36"/>
+      <c r="D17" s="35"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -4072,10 +4041,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="38"/>
+        <v>76</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="35"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -4083,10 +4052,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="38"/>
+        <v>75</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="D19" s="35"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -4094,10 +4063,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="38"/>
+        <v>149</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="35"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -4105,12 +4074,12 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="38"/>
+        <v>78</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="35"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -4118,10 +4087,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+        <v>79</v>
+      </c>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -4129,12 +4098,12 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="38"/>
+        <v>75</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="35"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -4142,10 +4111,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
+        <v>80</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -4153,10 +4122,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
+        <v>81</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -4164,10 +4133,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
+        <v>150</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -4175,12 +4144,12 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="38"/>
+        <v>114</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="35"/>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -4188,10 +4157,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
+        <v>115</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -4199,12 +4168,12 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="38"/>
+        <v>116</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="35"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -4212,10 +4181,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
+        <v>222</v>
+      </c>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4224,10 +4193,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
+        <v>92</v>
+      </c>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
@@ -4235,12 +4204,12 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="D32" s="38"/>
+        <v>119</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="35"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
@@ -4248,10 +4217,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="38"/>
+        <v>86</v>
+      </c>
+      <c r="C33" s="37"/>
+      <c r="D33" s="35"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -4259,12 +4228,12 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D34" s="38"/>
+        <v>118</v>
+      </c>
+      <c r="D34" s="35"/>
     </row>
     <row r="35" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
@@ -4272,12 +4241,12 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="D35" s="38"/>
+        <v>164</v>
+      </c>
+      <c r="D35" s="35"/>
     </row>
     <row r="36" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
@@ -4285,12 +4254,12 @@
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="D36" s="38"/>
+        <v>221</v>
+      </c>
+      <c r="D36" s="35"/>
     </row>
     <row r="37" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22">
@@ -4298,12 +4267,12 @@
         <v>36</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>233</v>
-      </c>
-      <c r="D37" s="38"/>
+        <v>225</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D37" s="35"/>
     </row>
     <row r="38" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
@@ -4311,10 +4280,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
+        <v>227</v>
+      </c>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
     </row>
     <row r="39" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
@@ -4322,12 +4291,12 @@
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39" s="38"/>
+        <v>157</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="35"/>
     </row>
     <row r="40" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
@@ -4335,10 +4304,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
+        <v>80</v>
+      </c>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
     </row>
     <row r="41" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22">
@@ -4346,12 +4315,12 @@
         <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="D41" s="38"/>
+      <c r="D41" s="35"/>
     </row>
     <row r="42" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
@@ -4359,13 +4328,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="D42" s="38" t="s">
-        <v>177</v>
+        <v>162</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4374,10 +4343,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
+        <v>163</v>
+      </c>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
@@ -4385,12 +4354,12 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="38"/>
+        <v>84</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="35"/>
     </row>
     <row r="45" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
@@ -4398,10 +4367,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
+        <v>105</v>
+      </c>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
     </row>
     <row r="46" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
@@ -4409,10 +4378,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
+        <v>106</v>
+      </c>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
@@ -4420,10 +4389,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
+        <v>107</v>
+      </c>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
@@ -4431,12 +4400,12 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>243</v>
-      </c>
-      <c r="C48" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="D48" s="38"/>
+        <v>236</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="35"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
@@ -4444,10 +4413,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
+        <v>237</v>
+      </c>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
@@ -4455,10 +4424,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
+        <v>43</v>
+      </c>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
@@ -4466,12 +4435,12 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="D51" s="38"/>
+        <v>230</v>
+      </c>
+      <c r="D51" s="35"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
@@ -4486,7 +4455,7 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
       <c r="C54" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D54" s="16"/>
     </row>
@@ -4543,63 +4512,63 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
it actually works now
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -3257,7 +3257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -3601,8 +3601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3817,8 +3817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4470,11 +4470,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D5:D41"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C42:C43"/>
     <mergeCell ref="C48:C50"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C9"/>
@@ -4486,6 +4481,11 @@
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C16:C20"/>
     <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D5:D41"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C42:C43"/>
     <mergeCell ref="D42:D51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
swap to 32-bit native arch with 64-bit extensions
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="281">
   <si>
     <t>Name</t>
   </si>
@@ -394,34 +394,10 @@
     <t>Integer Arithmetic 32bit</t>
   </si>
   <si>
-    <t>ADD32</t>
-  </si>
-  <si>
-    <t>SUB32</t>
-  </si>
-  <si>
-    <t>MUL32</t>
-  </si>
-  <si>
-    <t>DIV32</t>
-  </si>
-  <si>
-    <t>MOD32</t>
-  </si>
-  <si>
-    <t>SHL32</t>
-  </si>
-  <si>
     <t>MULU</t>
   </si>
   <si>
     <t>DIVU</t>
-  </si>
-  <si>
-    <t>MULU32</t>
-  </si>
-  <si>
-    <t>DIVU32</t>
   </si>
   <si>
     <t>Float Arithmetic 32bit</t>
@@ -465,18 +441,6 @@
     </r>
   </si>
   <si>
-    <t>MOV32</t>
-  </si>
-  <si>
-    <t>PUSH32</t>
-  </si>
-  <si>
-    <t>POP32</t>
-  </si>
-  <si>
-    <t>SP -= 2, Reg = RAM[SP]</t>
-  </si>
-  <si>
     <t>SP -= 4, Reg = RAM[SP]</t>
   </si>
   <si>
@@ -570,12 +534,6 @@
     <t>POPREG</t>
   </si>
   <si>
-    <t>PUSH32 $R12; PUSH32 $R34</t>
-  </si>
-  <si>
-    <t>POP32 $R34; POP32 $R12</t>
-  </si>
-  <si>
     <t>stdout (return)</t>
   </si>
   <si>
@@ -669,12 +627,6 @@
     <t>CR = COMPARE_FLOAT(Reg, Reg2)</t>
   </si>
   <si>
-    <t>CMP32</t>
-  </si>
-  <si>
-    <t>CR = COMPARE_32BIT(Reg, Reg2)</t>
-  </si>
-  <si>
     <t>Compare</t>
   </si>
   <si>
@@ -690,9 +642,6 @@
     <t>CMPS</t>
   </si>
   <si>
-    <t>CMP32S</t>
-  </si>
-  <si>
     <t>MREGC</t>
   </si>
   <si>
@@ -703,9 +652,6 @@
   </si>
   <si>
     <t>JG</t>
-  </si>
-  <si>
-    <t>LSHR32</t>
   </si>
   <si>
     <t>Overwirte ROM encryption key in RAM with 0</t>
@@ -770,30 +716,12 @@
     <t>JNZ $ENCREG2,51</t>
   </si>
   <si>
-    <t>ID = POP; PUSH32es I/O write pointer for ID</t>
-  </si>
-  <si>
-    <t>ID = POP; PUSH32es I/O read pointer for ID</t>
-  </si>
-  <si>
-    <t>ID = POP; PUSH32es I/O length for ID (or -1 if not available)</t>
-  </si>
-  <si>
-    <t>ID = POP; Offset =POP32; Sets I/O write pointer for ID to Offset</t>
-  </si>
-  <si>
-    <t>ID = POP; Offset =POP32; Sets I/O read pointer for ID to Offset</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
     <t>RRVV</t>
   </si>
   <si>
-    <t>RRVV32</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -809,9 +737,6 @@
     <t>RegDst = RegSrc</t>
   </si>
   <si>
-    <t>RAM[SP] = Reg, SP += 2</t>
-  </si>
-  <si>
     <t>RAM[SP] = Reg, SP += 4</t>
   </si>
   <si>
@@ -869,24 +794,12 @@
     <t>Reg != 0 -&gt; PC = Reg2</t>
   </si>
   <si>
-    <t>CALL RAM[IHBASE+Reg*2]</t>
-  </si>
-  <si>
-    <t>RAM[IHBASE+Reg*2] = Reg2 (0 for disable)</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
-    <t>SP -= 2, PC = RAM[SP]</t>
-  </si>
-  <si>
     <t>ASHR</t>
   </si>
   <si>
-    <t>ASHR32</t>
-  </si>
-  <si>
     <t>If trap set after next instruction, unsets trap, PUSH $PC</t>
   </si>
   <si>
@@ -903,6 +816,96 @@
   </si>
   <si>
     <t>MOV8</t>
+  </si>
+  <si>
+    <t>ADD64</t>
+  </si>
+  <si>
+    <t>SUB64</t>
+  </si>
+  <si>
+    <t>MUL64</t>
+  </si>
+  <si>
+    <t>DIV64</t>
+  </si>
+  <si>
+    <t>MOD64</t>
+  </si>
+  <si>
+    <t>SHL64</t>
+  </si>
+  <si>
+    <t>LSHR64</t>
+  </si>
+  <si>
+    <t>ASHR64</t>
+  </si>
+  <si>
+    <t>MULU64</t>
+  </si>
+  <si>
+    <t>DIVU64</t>
+  </si>
+  <si>
+    <t>RRVV64</t>
+  </si>
+  <si>
+    <t>CMP64</t>
+  </si>
+  <si>
+    <t>CMP64S</t>
+  </si>
+  <si>
+    <t>CR = COMPARE_64BIT(Reg, Reg2)</t>
+  </si>
+  <si>
+    <t>PUSH64</t>
+  </si>
+  <si>
+    <t>MOV64</t>
+  </si>
+  <si>
+    <t>POP64</t>
+  </si>
+  <si>
+    <t>PUSH64 $R12; PUSH64 $R34</t>
+  </si>
+  <si>
+    <t>POP64 $R34; POP64 $R12</t>
+  </si>
+  <si>
+    <t>RAM[SP] = Reg, SP += 8</t>
+  </si>
+  <si>
+    <t>SP -= 8, Reg = RAM[SP]</t>
+  </si>
+  <si>
+    <t>SP -= 4, PC = RAM[SP]</t>
+  </si>
+  <si>
+    <t>CALL RAM[IHBASE+Reg*4]</t>
+  </si>
+  <si>
+    <t>RAM[IHBASE+Reg*4] = Reg2 (0 for disable)</t>
+  </si>
+  <si>
+    <t>ID = POP; Offset =POP; Sets I/O write pointer for ID to Offset</t>
+  </si>
+  <si>
+    <t>ID = POP; Offset =POP; Sets I/O read pointer for ID to Offset</t>
+  </si>
+  <si>
+    <t>ID = POP; PUSHes I/O write pointer for ID</t>
+  </si>
+  <si>
+    <t>ID = POP; PUSHes I/O read pointer for ID</t>
+  </si>
+  <si>
+    <t>ID = POP; PUSHes I/O length for ID (or -1 if not available)</t>
+  </si>
+  <si>
+    <t>MOV16</t>
   </si>
 </sst>
 </file>
@@ -1082,6 +1085,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1094,7 +1098,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1414,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74:H74"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74:G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,7 +1434,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1440,16 +1443,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -1470,7 +1473,7 @@
         <v>00</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -1479,13 +1482,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>137</v>
+        <v>266</v>
       </c>
       <c r="C3" s="2">
         <f>C2+1</f>
@@ -1496,7 +1499,7 @@
         <v>01</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
@@ -1505,7 +1508,7 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1521,13 +1524,13 @@
         <v>02</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F4" t="s">
         <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1543,19 +1546,19 @@
         <v>03</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>138</v>
+        <v>265</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="1"/>
@@ -1566,19 +1569,19 @@
         <v>04</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>249</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>139</v>
+        <v>267</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
@@ -1589,13 +1592,13 @@
         <v>05</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>141</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1611,7 +1614,7 @@
         <v>06</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1630,7 +1633,7 @@
         <v>07</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -1639,7 +1642,7 @@
         <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1655,7 +1658,7 @@
         <v>08</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
@@ -1664,7 +1667,7 @@
         <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1680,7 +1683,7 @@
         <v>09</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -1689,7 +1692,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1705,7 +1708,7 @@
         <v>0A</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -1714,7 +1717,7 @@
         <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1730,7 +1733,7 @@
         <v>0B</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -1739,7 +1742,7 @@
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1755,7 +1758,7 @@
         <v>0C</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -1764,12 +1767,12 @@
         <v>16</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
@@ -1780,7 +1783,7 @@
         <v>0D</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
@@ -1789,12 +1792,12 @@
         <v>16</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="1"/>
@@ -1805,7 +1808,7 @@
         <v>0E</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>17</v>
@@ -1814,12 +1817,12 @@
         <v>16</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
@@ -1830,7 +1833,7 @@
         <v>0F</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>17</v>
@@ -1839,12 +1842,12 @@
         <v>16</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
@@ -1855,7 +1858,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
@@ -1864,7 +1867,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1883,7 +1886,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -1892,7 +1895,7 @@
         <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1908,7 +1911,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
@@ -1917,7 +1920,7 @@
         <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1933,7 +1936,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -1942,7 +1945,7 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1959,7 +1962,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>17</v>
@@ -1968,7 +1971,7 @@
         <v>16</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1987,7 +1990,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>17</v>
@@ -1996,7 +1999,7 @@
         <v>16</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2015,7 +2018,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
@@ -2024,17 +2027,17 @@
         <v>16</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="C25" s="22">
         <f t="shared" si="1"/>
@@ -2045,7 +2048,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F25" s="22" t="s">
         <v>28</v>
@@ -2054,12 +2057,12 @@
         <v>33</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="C26" s="22">
         <f t="shared" si="1"/>
@@ -2070,7 +2073,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F26" s="22" t="s">
         <v>28</v>
@@ -2082,7 +2085,7 @@
     <row r="27" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29"/>
       <c r="B27" s="22" t="s">
-        <v>205</v>
+        <v>262</v>
       </c>
       <c r="C27" s="22">
         <f t="shared" si="1"/>
@@ -2093,7 +2096,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F27" s="22" t="s">
         <v>28</v>
@@ -2102,13 +2105,13 @@
         <v>33</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>206</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30"/>
       <c r="B28" s="22" t="s">
-        <v>212</v>
+        <v>263</v>
       </c>
       <c r="C28" s="22">
         <f t="shared" si="1"/>
@@ -2119,7 +2122,7 @@
         <v>1A</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F28" s="22" t="s">
         <v>28</v>
@@ -2130,7 +2133,7 @@
     </row>
     <row r="29" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="22" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C29" s="22">
         <f t="shared" si="1"/>
@@ -2141,7 +2144,7 @@
         <v>1B</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="F29" s="22" t="s">
         <v>28</v>
@@ -2150,7 +2153,7 @@
         <v>33</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2169,21 +2172,21 @@
         <v>1C</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F30" s="22" t="s">
         <v>28</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="2" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="1"/>
@@ -2194,7 +2197,7 @@
         <v>1D</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>28</v>
@@ -2207,7 +2210,7 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="1"/>
@@ -2218,7 +2221,7 @@
         <v>1E</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>28</v>
@@ -2242,7 +2245,7 @@
         <v>1F</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F33" s="22" t="s">
         <v>28</v>
@@ -2266,7 +2269,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F34" s="22" t="s">
         <v>28</v>
@@ -2278,7 +2281,7 @@
     </row>
     <row r="35" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="22" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="C35" s="22">
         <f t="shared" si="1"/>
@@ -2289,7 +2292,7 @@
         <v>21</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F35" s="22" t="s">
         <v>28</v>
@@ -2299,7 +2302,7 @@
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C36" s="22">
         <f t="shared" si="1"/>
@@ -2310,7 +2313,7 @@
         <v>22</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>28</v>
@@ -2334,7 +2337,7 @@
         <v>23</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>28</v>
@@ -2343,7 +2346,7 @@
         <v>33</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -2362,7 +2365,7 @@
         <v>24</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>28</v>
@@ -2371,7 +2374,7 @@
         <v>33</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -2390,7 +2393,7 @@
         <v>25</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F39" s="22" t="s">
         <v>28</v>
@@ -2399,14 +2402,14 @@
       <c r="H39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J39" s="36" t="s">
-        <v>136</v>
+      <c r="J39" s="37" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="C40" s="2">
         <f t="shared" si="1"/>
@@ -2417,7 +2420,7 @@
         <v>26</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>28</v>
@@ -2425,12 +2428,12 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="36"/>
+      <c r="J40" s="37"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="C41" s="2">
         <f t="shared" si="1"/>
@@ -2441,7 +2444,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>28</v>
@@ -2449,7 +2452,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="36"/>
+      <c r="J41" s="37"/>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -2465,7 +2468,7 @@
         <v>28</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F42" s="22" t="s">
         <v>28</v>
@@ -2473,7 +2476,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="36"/>
+      <c r="J42" s="37"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -2489,7 +2492,7 @@
         <v>29</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F43" s="22" t="s">
         <v>28</v>
@@ -2497,12 +2500,12 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="36"/>
+      <c r="J43" s="37"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C44" s="2">
         <f t="shared" si="1"/>
@@ -2513,7 +2516,7 @@
         <v>2A</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>28</v>
@@ -2521,12 +2524,12 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="36"/>
+      <c r="J44" s="37"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="C45" s="2">
         <f t="shared" si="1"/>
@@ -2537,7 +2540,7 @@
         <v>2B</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>28</v>
@@ -2545,7 +2548,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="36"/>
+      <c r="J45" s="37"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
@@ -2561,7 +2564,7 @@
         <v>2C</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>28</v>
@@ -2570,10 +2573,10 @@
         <v>33</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="I46" s="2"/>
-      <c r="J46" s="36"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
@@ -2589,7 +2592,7 @@
         <v>2D</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>28</v>
@@ -2598,10 +2601,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="I47" s="2"/>
-      <c r="J47" s="36"/>
+      <c r="J47" s="37"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
@@ -2617,12 +2620,12 @@
         <v>2E</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -2643,14 +2646,14 @@
         <v>2F</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F49" s="22" t="s">
         <v>28</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="2" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -2669,7 +2672,7 @@
         <v>30</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F50" s="22" t="s">
         <v>28</v>
@@ -2678,7 +2681,7 @@
         <v>33</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2697,7 +2700,7 @@
         <v>31</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -2721,7 +2724,7 @@
         <v>32</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -2745,7 +2748,7 @@
         <v>33</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -2757,7 +2760,7 @@
     </row>
     <row r="54" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C54" s="15">
         <f t="shared" si="1"/>
@@ -2768,15 +2771,15 @@
         <v>34</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="15" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C55" s="15">
         <f t="shared" si="1"/>
@@ -2787,15 +2790,15 @@
         <v>35</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="17" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C56" s="17">
         <f t="shared" si="1"/>
@@ -2806,15 +2809,15 @@
         <v>36</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>172</v>
+        <v>268</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="17" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C57" s="17">
         <f t="shared" si="1"/>
@@ -2825,15 +2828,15 @@
         <v>37</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>173</v>
+        <v>269</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="22" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="C58" s="22">
         <f t="shared" si="1"/>
@@ -2844,10 +2847,10 @@
         <v>38</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="H58" s="22" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -2855,7 +2858,7 @@
         <v>120</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>121</v>
+        <v>251</v>
       </c>
       <c r="C59" s="22">
         <f t="shared" si="1"/>
@@ -2866,7 +2869,7 @@
         <v>39</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>17</v>
@@ -2875,13 +2878,13 @@
         <v>16</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="2" t="s">
-        <v>122</v>
+        <v>252</v>
       </c>
       <c r="C60" s="2">
         <f t="shared" si="1"/>
@@ -2892,7 +2895,7 @@
         <v>3A</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>17</v>
@@ -2901,13 +2904,13 @@
         <v>16</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" s="2" t="s">
-        <v>123</v>
+        <v>253</v>
       </c>
       <c r="C61" s="2">
         <f t="shared" si="1"/>
@@ -2918,7 +2921,7 @@
         <v>3B</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>17</v>
@@ -2927,13 +2930,13 @@
         <v>16</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" s="2" t="s">
-        <v>124</v>
+        <v>254</v>
       </c>
       <c r="C62" s="2">
         <f t="shared" si="1"/>
@@ -2944,7 +2947,7 @@
         <v>3C</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>17</v>
@@ -2953,13 +2956,13 @@
         <v>16</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="2" t="s">
-        <v>125</v>
+        <v>255</v>
       </c>
       <c r="C63" s="2">
         <f t="shared" si="1"/>
@@ -2970,7 +2973,7 @@
         <v>3D</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>17</v>
@@ -2979,13 +2982,13 @@
         <v>16</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="2" t="s">
-        <v>126</v>
+        <v>256</v>
       </c>
       <c r="C64" s="2">
         <f t="shared" si="1"/>
@@ -2996,7 +2999,7 @@
         <v>3E</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>17</v>
@@ -3005,13 +3008,13 @@
         <v>16</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="2" t="s">
-        <v>217</v>
+        <v>257</v>
       </c>
       <c r="C65" s="2">
         <f t="shared" si="1"/>
@@ -3022,7 +3025,7 @@
         <v>3F</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>17</v>
@@ -3031,13 +3034,13 @@
         <v>16</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="2" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="C66" s="2">
         <f t="shared" si="1"/>
@@ -3048,7 +3051,7 @@
         <v>40</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>17</v>
@@ -3057,13 +3060,13 @@
         <v>16</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="2" t="s">
-        <v>129</v>
+        <v>259</v>
       </c>
       <c r="C67" s="2">
         <f t="shared" si="1"/>
@@ -3074,7 +3077,7 @@
         <v>41</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>17</v>
@@ -3083,13 +3086,13 @@
         <v>16</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="2" t="s">
-        <v>130</v>
+        <v>260</v>
       </c>
       <c r="C68" s="2">
         <f t="shared" si="1"/>
@@ -3100,7 +3103,7 @@
         <v>42</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>17</v>
@@ -3109,15 +3112,15 @@
         <v>16</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B69" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C69" s="2">
         <f t="shared" si="1"/>
@@ -3128,7 +3131,7 @@
         <v>43</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>17</v>
@@ -3137,13 +3140,13 @@
         <v>16</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C70" s="2">
         <f t="shared" si="1"/>
@@ -3154,7 +3157,7 @@
         <v>44</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>17</v>
@@ -3163,13 +3166,13 @@
         <v>16</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C71" s="2">
         <f t="shared" si="1"/>
@@ -3180,7 +3183,7 @@
         <v>45</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>17</v>
@@ -3189,13 +3192,13 @@
         <v>16</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C72" s="2">
         <f t="shared" si="1"/>
@@ -3206,7 +3209,7 @@
         <v>46</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>17</v>
@@ -3215,13 +3218,13 @@
         <v>16</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="B73" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="C73" s="22">
         <f t="shared" si="1"/>
@@ -3232,7 +3235,7 @@
         <v>47</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F73" t="s">
         <v>17</v>
@@ -3243,12 +3246,26 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="35"/>
-      <c r="B74" s="40"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="22"/>
-      <c r="G74" s="22"/>
+      <c r="B74" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="C74" s="22">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="D74" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F74" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G74" s="22" t="s">
+        <v>16</v>
+      </c>
       <c r="H74" s="35"/>
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3257,7 +3274,6 @@
       <c r="C75" s="34"/>
       <c r="D75" s="34"/>
       <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
       <c r="G75" s="34"/>
       <c r="H75" s="34"/>
     </row>
@@ -3287,7 +3303,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3347,7 +3363,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>238</v>
+        <v>275</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
@@ -3362,7 +3378,7 @@
         <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>239</v>
+        <v>276</v>
       </c>
       <c r="D5" t="s">
         <v>61</v>
@@ -3377,7 +3393,7 @@
         <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>235</v>
+        <v>277</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -3392,7 +3408,7 @@
         <v>67</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="D7" t="s">
         <v>61</v>
@@ -3407,7 +3423,7 @@
         <v>68</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -3438,10 +3454,10 @@
         <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>60</v>
@@ -3456,7 +3472,7 @@
         <v>53</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="D12" t="s">
         <v>60</v>
@@ -3471,7 +3487,7 @@
         <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="D13" t="s">
         <v>60</v>
@@ -3514,22 +3530,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3537,17 +3553,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
       <c r="E2" s="25"/>
       <c r="F2" s="23" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="G2" s="23"/>
       <c r="I2" s="26" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3556,7 +3572,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="23"/>
@@ -3564,7 +3580,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="I3" s="27" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3573,7 +3589,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="23"/>
@@ -3581,7 +3597,7 @@
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
       <c r="I4" s="28" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3590,18 +3606,18 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="23" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="23" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3610,13 +3626,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="23" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="G6" s="23"/>
     </row>
@@ -3631,7 +3647,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:D9"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3657,10 +3673,10 @@
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="38" t="s">
+      <c r="C2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3672,8 +3688,8 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3683,10 +3699,10 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" s="38"/>
+      <c r="C4" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="39"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3696,8 +3712,8 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="39"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3705,7 +3721,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -3717,10 +3733,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3741,10 +3757,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3753,13 +3769,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="C10" s="37" t="s">
-        <v>192</v>
+        <v>130</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>178</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,9 +3784,9 @@
         <v>9</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="C11" s="37"/>
+        <v>131</v>
+      </c>
+      <c r="C11" s="38"/>
       <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3816,10 +3832,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="D16" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3828,10 +3844,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3856,8 +3872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B51"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3879,7 +3895,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3887,12 +3903,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="37"/>
+        <v>139</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -3900,10 +3916,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
+        <v>140</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
     </row>
     <row r="4" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
@@ -3911,10 +3927,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+        <v>144</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
@@ -3922,12 +3938,12 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="37"/>
+        <v>210</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="38"/>
       <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3936,10 +3952,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+        <v>211</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3948,10 +3964,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+        <v>212</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3960,10 +3976,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+        <v>213</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="22"/>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3972,10 +3988,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+        <v>214</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3989,7 +4005,7 @@
       <c r="C10" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="38"/>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -4002,7 +4018,7 @@
       <c r="C11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="37"/>
+      <c r="D11" s="38"/>
     </row>
     <row r="12" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
@@ -4012,10 +4028,10 @@
       <c r="B12" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="37"/>
+      <c r="D12" s="38"/>
     </row>
     <row r="13" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
@@ -4025,8 +4041,8 @@
       <c r="B13" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
@@ -4036,8 +4052,8 @@
       <c r="B14" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
@@ -4047,8 +4063,8 @@
       <c r="B15" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
     </row>
     <row r="16" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
@@ -4058,10 +4074,10 @@
       <c r="B16" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="37"/>
+      <c r="D16" s="38"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
@@ -4069,10 +4085,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="37"/>
+        <v>134</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -4082,8 +4098,8 @@
       <c r="B18" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="37"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="38"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -4093,8 +4109,8 @@
       <c r="B19" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="37"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="38"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -4102,10 +4118,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
-      </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="37"/>
+        <v>135</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="38"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -4115,10 +4131,10 @@
       <c r="B21" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="37"/>
+      <c r="D21" s="38"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -4128,8 +4144,8 @@
       <c r="B22" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -4139,10 +4155,10 @@
       <c r="B23" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="37"/>
+      <c r="D23" s="38"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -4152,8 +4168,8 @@
       <c r="B24" t="s">
         <v>79</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -4163,8 +4179,8 @@
       <c r="B25" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -4172,10 +4188,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
-      </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
+        <v>136</v>
+      </c>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -4185,10 +4201,10 @@
       <c r="B27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="37"/>
+      <c r="D27" s="38"/>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -4198,8 +4214,8 @@
       <c r="B28" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -4209,10 +4225,10 @@
       <c r="B29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="37"/>
+      <c r="D29" s="38"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -4220,10 +4236,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
+        <v>201</v>
+      </c>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4234,8 +4250,8 @@
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
@@ -4245,10 +4261,10 @@
       <c r="B32" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="37"/>
+      <c r="D32" s="38"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
@@ -4258,8 +4274,8 @@
       <c r="B33" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="37"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="38"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -4272,7 +4288,7 @@
       <c r="C34" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="37"/>
+      <c r="D34" s="38"/>
     </row>
     <row r="35" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
@@ -4280,12 +4296,12 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="D35" s="37"/>
+        <v>150</v>
+      </c>
+      <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
@@ -4293,12 +4309,12 @@
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="D36" s="37"/>
+        <v>200</v>
+      </c>
+      <c r="D36" s="38"/>
     </row>
     <row r="37" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22">
@@ -4306,12 +4322,12 @@
         <v>36</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="C37" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="D37" s="37"/>
+        <v>204</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="D37" s="38"/>
     </row>
     <row r="38" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
@@ -4319,10 +4335,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
+        <v>206</v>
+      </c>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
     </row>
     <row r="39" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
@@ -4330,12 +4346,12 @@
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C39" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="D39" s="37"/>
+        <v>143</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="38"/>
     </row>
     <row r="40" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
@@ -4345,8 +4361,8 @@
       <c r="B40" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
     </row>
     <row r="41" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22">
@@ -4354,12 +4370,12 @@
         <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D41" s="37"/>
+        <v>152</v>
+      </c>
+      <c r="D41" s="38"/>
     </row>
     <row r="42" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
@@ -4367,13 +4383,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C42" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="D42" s="37" t="s">
-        <v>168</v>
+        <v>148</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" s="38" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4382,10 +4398,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
+        <v>149</v>
+      </c>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
@@ -4395,10 +4411,10 @@
       <c r="B44" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="37"/>
+      <c r="D44" s="38"/>
     </row>
     <row r="45" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
@@ -4408,8 +4424,8 @@
       <c r="B45" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
     </row>
     <row r="46" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
@@ -4419,8 +4435,8 @@
       <c r="B46" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
@@ -4430,8 +4446,8 @@
       <c r="B47" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
@@ -4439,12 +4455,12 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>233</v>
-      </c>
-      <c r="C48" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D48" s="37"/>
+        <v>215</v>
+      </c>
+      <c r="C48" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48" s="38"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
@@ -4452,10 +4468,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
+        <v>216</v>
+      </c>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
@@ -4465,8 +4481,8 @@
       <c r="B50" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
@@ -4474,12 +4490,12 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="D51" s="37"/>
+        <v>209</v>
+      </c>
+      <c r="D51" s="38"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
@@ -4509,6 +4525,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C39:C40"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="D42:D51"/>
     <mergeCell ref="C48:C50"/>
@@ -4525,7 +4542,6 @@
     <mergeCell ref="D5:D41"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C39:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
up RAM size to 4MB
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="282">
   <si>
     <t>Name</t>
   </si>
@@ -906,6 +906,9 @@
   </si>
   <si>
     <t>MOV16</t>
+  </si>
+  <si>
+    <t>DEBUG</t>
   </si>
 </sst>
 </file>
@@ -1417,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74:G74"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1541,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:C74" si="1">C4+1</f>
+        <f t="shared" ref="C5:C75" si="1">C4+1</f>
         <v>3</v>
       </c>
       <c r="D5" s="19" t="str">
@@ -3179,7 +3182,7 @@
         <v>69</v>
       </c>
       <c r="D71" s="19" t="str">
-        <f t="shared" ref="D71:D74" si="3">DEC2HEX(C71,2)</f>
+        <f t="shared" ref="D71:D75" si="3">DEC2HEX(C71,2)</f>
         <v>45</v>
       </c>
       <c r="E71" s="10" t="s">
@@ -3270,10 +3273,20 @@
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="34"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
+      <c r="B75" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="C75" s="22">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="D75" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>219</v>
+      </c>
       <c r="G75" s="34"/>
       <c r="H75" s="34"/>
     </row>
@@ -4525,6 +4538,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D2:D4"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="D42:D51"/>
@@ -4541,7 +4555,6 @@
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="D5:D41"/>
     <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D2:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
spaces->tabs. also flagr stuff
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="303">
   <si>
     <t>Name</t>
   </si>
@@ -627,12 +627,6 @@
     <t>Compare</t>
   </si>
   <si>
-    <t>FLAGR</t>
-  </si>
-  <si>
-    <t>Flag register</t>
-  </si>
-  <si>
     <t>MREG</t>
   </si>
   <si>
@@ -942,6 +936,42 @@
   </si>
   <si>
     <t>Extra</t>
+  </si>
+  <si>
+    <t>MSR</t>
+  </si>
+  <si>
+    <t>Internal CPU register</t>
+  </si>
+  <si>
+    <t>SOFF1</t>
+  </si>
+  <si>
+    <t>SOFF2</t>
+  </si>
+  <si>
+    <t>SOFF12</t>
+  </si>
+  <si>
+    <t>Off1</t>
+  </si>
+  <si>
+    <t>Off2</t>
+  </si>
+  <si>
+    <t>R1OFFSET = Off1</t>
+  </si>
+  <si>
+    <t>R2OFFSET = Off2</t>
+  </si>
+  <si>
+    <t>R1OFFET = Off1; R2OFFSET = Off2</t>
+  </si>
+  <si>
+    <t>V8</t>
+  </si>
+  <si>
+    <t>V8V8</t>
   </si>
 </sst>
 </file>
@@ -1449,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,7 +1496,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1478,13 +1508,13 @@
         <v>156</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -1505,7 +1535,7 @@
         <v>00</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -1514,13 +1544,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C3" s="2">
         <f>C2+1</f>
@@ -1531,7 +1561,7 @@
         <v>01</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
@@ -1540,13 +1570,13 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C4" s="21">
         <f>C3+1</f>
@@ -1557,7 +1587,7 @@
         <v>02</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -1566,13 +1596,13 @@
         <v>16</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C5" s="21">
         <f>C4+1</f>
@@ -1583,7 +1613,7 @@
         <v>03</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>17</v>
@@ -1592,7 +1622,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1608,13 +1638,13 @@
         <v>04</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1622,7 +1652,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" ref="C7:C81" si="1">C6+1</f>
+        <f t="shared" ref="C7:C83" si="1">C6+1</f>
         <v>5</v>
       </c>
       <c r="D7" s="18" t="str">
@@ -1630,7 +1660,7 @@
         <v>05</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F7" t="s">
         <v>28</v>
@@ -1642,7 +1672,7 @@
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
@@ -1653,19 +1683,19 @@
         <v>06</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
@@ -1676,13 +1706,13 @@
         <v>07</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1698,7 +1728,7 @@
         <v>08</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1717,7 +1747,7 @@
         <v>09</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -1726,7 +1756,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1742,7 +1772,7 @@
         <v>0A</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -1751,7 +1781,7 @@
         <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1767,7 +1797,7 @@
         <v>0B</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -1776,7 +1806,7 @@
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,7 +1822,7 @@
         <v>0C</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -1801,7 +1831,7 @@
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1817,7 +1847,7 @@
         <v>0D</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -1826,7 +1856,7 @@
         <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1842,7 +1872,7 @@
         <v>0E</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -1851,7 +1881,7 @@
         <v>16</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1867,7 +1897,7 @@
         <v>0F</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>17</v>
@@ -1876,12 +1906,12 @@
         <v>16</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
@@ -1892,7 +1922,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
@@ -1901,7 +1931,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1917,7 +1947,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>17</v>
@@ -1926,7 +1956,7 @@
         <v>16</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1942,7 +1972,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>17</v>
@@ -1951,7 +1981,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1970,7 +2000,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -1979,7 +2009,7 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1995,7 +2025,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
@@ -2004,7 +2034,7 @@
         <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2020,7 +2050,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -2029,7 +2059,7 @@
         <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2046,7 +2076,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
@@ -2055,7 +2085,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2074,7 +2104,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>17</v>
@@ -2083,7 +2113,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2102,7 +2132,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>17</v>
@@ -2111,7 +2141,7 @@
         <v>16</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2132,7 +2162,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>28</v>
@@ -2146,7 +2176,7 @@
     </row>
     <row r="28" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C28" s="21">
         <f t="shared" si="1"/>
@@ -2157,7 +2187,7 @@
         <v>1A</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>28</v>
@@ -2169,7 +2199,7 @@
     <row r="29" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C29" s="21">
         <f t="shared" si="1"/>
@@ -2180,7 +2210,7 @@
         <v>1B</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>28</v>
@@ -2189,13 +2219,13 @@
         <v>33</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
       <c r="B30" s="21" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C30" s="21">
         <f t="shared" si="1"/>
@@ -2206,7 +2236,7 @@
         <v>1C</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>28</v>
@@ -2228,7 +2258,7 @@
         <v>1D</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>28</v>
@@ -2242,7 +2272,7 @@
     </row>
     <row r="32" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="21" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C32" s="21">
         <f t="shared" si="1"/>
@@ -2253,7 +2283,7 @@
         <v>1E</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>28</v>
@@ -2262,7 +2292,7 @@
         <v>33</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2281,14 +2311,14 @@
         <v>1F</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J33" s="3"/>
     </row>
@@ -2306,7 +2336,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>28</v>
@@ -2330,7 +2360,7 @@
         <v>21</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>28</v>
@@ -2354,7 +2384,7 @@
         <v>22</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F36" s="21" t="s">
         <v>28</v>
@@ -2378,7 +2408,7 @@
         <v>23</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>28</v>
@@ -2390,7 +2420,7 @@
     </row>
     <row r="38" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C38" s="21">
         <f t="shared" si="1"/>
@@ -2401,7 +2431,7 @@
         <v>24</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F38" s="21" t="s">
         <v>28</v>
@@ -2422,7 +2452,7 @@
         <v>25</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>28</v>
@@ -2446,7 +2476,7 @@
         <v>26</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>28</v>
@@ -2455,7 +2485,7 @@
         <v>33</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2474,7 +2504,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>28</v>
@@ -2483,7 +2513,7 @@
         <v>33</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2502,7 +2532,7 @@
         <v>28</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>28</v>
@@ -2529,7 +2559,7 @@
         <v>29</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>28</v>
@@ -2553,7 +2583,7 @@
         <v>2A</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>28</v>
@@ -2577,7 +2607,7 @@
         <v>2B</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>28</v>
@@ -2601,7 +2631,7 @@
         <v>2C</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>28</v>
@@ -2625,7 +2655,7 @@
         <v>2D</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>28</v>
@@ -2649,7 +2679,7 @@
         <v>2E</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>28</v>
@@ -2673,7 +2703,7 @@
         <v>2F</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>28</v>
@@ -2682,7 +2712,7 @@
         <v>33</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="35"/>
@@ -2701,7 +2731,7 @@
         <v>30</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>28</v>
@@ -2710,7 +2740,7 @@
         <v>33</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="35"/>
@@ -2729,12 +2759,12 @@
         <v>31</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2755,14 +2785,14 @@
         <v>32</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F52" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G52" s="21"/>
       <c r="H52" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2781,7 +2811,7 @@
         <v>33</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>28</v>
@@ -2790,7 +2820,7 @@
         <v>33</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2809,7 +2839,7 @@
         <v>34</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -2833,7 +2863,7 @@
         <v>35</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -2857,7 +2887,7 @@
         <v>36</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -2880,7 +2910,7 @@
         <v>37</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H57" s="14" t="s">
         <v>146</v>
@@ -2899,7 +2929,7 @@
         <v>38</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H58" s="14" t="s">
         <v>145</v>
@@ -2918,10 +2948,10 @@
         <v>39</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2937,15 +2967,15 @@
         <v>3A</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C61" s="21">
         <f t="shared" si="1"/>
@@ -2956,18 +2986,18 @@
         <v>3B</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C62" s="21">
         <f>C61+1</f>
@@ -2978,7 +3008,7 @@
         <v>3C</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>17</v>
@@ -2987,13 +3017,13 @@
         <v>16</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C63" s="2">
         <f t="shared" si="1"/>
@@ -3004,7 +3034,7 @@
         <v>3D</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>17</v>
@@ -3013,13 +3043,13 @@
         <v>16</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C64" s="2">
         <f t="shared" si="1"/>
@@ -3030,7 +3060,7 @@
         <v>3E</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>17</v>
@@ -3039,13 +3069,13 @@
         <v>16</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C65" s="2">
         <f t="shared" si="1"/>
@@ -3056,7 +3086,7 @@
         <v>3F</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>17</v>
@@ -3065,13 +3095,13 @@
         <v>16</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C66" s="2">
         <f t="shared" si="1"/>
@@ -3082,7 +3112,7 @@
         <v>40</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>17</v>
@@ -3091,13 +3121,13 @@
         <v>16</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C67" s="2">
         <f t="shared" si="1"/>
@@ -3108,7 +3138,7 @@
         <v>41</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>17</v>
@@ -3117,13 +3147,13 @@
         <v>16</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C68" s="2">
         <f t="shared" si="1"/>
@@ -3134,7 +3164,7 @@
         <v>42</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>17</v>
@@ -3143,13 +3173,13 @@
         <v>16</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C69" s="2">
         <f t="shared" si="1"/>
@@ -3160,7 +3190,7 @@
         <v>43</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>17</v>
@@ -3169,24 +3199,24 @@
         <v>16</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="D70" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E70" s="10" t="s">
         <v>258</v>
-      </c>
-      <c r="C70" s="2">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="D70" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>260</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>17</v>
@@ -3195,13 +3225,13 @@
         <v>16</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C71" s="2">
         <f t="shared" si="1"/>
@@ -3212,7 +3242,7 @@
         <v>45</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>17</v>
@@ -3221,7 +3251,7 @@
         <v>16</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3240,7 +3270,7 @@
         <v>46</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>17</v>
@@ -3249,7 +3279,7 @@
         <v>16</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3266,7 +3296,7 @@
         <v>47</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>17</v>
@@ -3275,7 +3305,7 @@
         <v>16</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3292,7 +3322,7 @@
         <v>48</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>17</v>
@@ -3301,7 +3331,7 @@
         <v>16</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3318,7 +3348,7 @@
         <v>49</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>17</v>
@@ -3327,15 +3357,15 @@
         <v>16</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C76" s="21">
         <f t="shared" si="1"/>
@@ -3346,7 +3376,7 @@
         <v>4A</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F76" s="21" t="s">
         <v>17</v>
@@ -3355,13 +3385,13 @@
         <v>16</v>
       </c>
       <c r="H76" s="21" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="B77" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C77" s="21">
         <f t="shared" si="1"/>
@@ -3372,7 +3402,7 @@
         <v>4B</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F77" s="21" t="s">
         <v>17</v>
@@ -3381,13 +3411,13 @@
         <v>16</v>
       </c>
       <c r="H77" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="B78" s="21" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C78" s="21">
         <f t="shared" si="1"/>
@@ -3398,7 +3428,7 @@
         <v>4C</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F78" s="21" t="s">
         <v>17</v>
@@ -3407,13 +3437,13 @@
         <v>16</v>
       </c>
       <c r="H78" s="21" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="B79" s="21" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C79" s="21">
         <f t="shared" si="1"/>
@@ -3424,7 +3454,7 @@
         <v>4D</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F79" s="21" t="s">
         <v>17</v>
@@ -3433,15 +3463,15 @@
         <v>16</v>
       </c>
       <c r="H79" s="21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="32" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B80" s="32" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C80" s="21">
         <f t="shared" si="1"/>
@@ -3452,38 +3482,82 @@
         <v>4E</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
-      <c r="B81" s="21"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="21"/>
+      <c r="B81" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="C81" s="21">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="D81" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>4F</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F81" s="21" t="s">
+        <v>296</v>
+      </c>
       <c r="G81" s="21"/>
-      <c r="H81" s="21"/>
+      <c r="H81" s="21" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="21"/>
+      <c r="B82" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C82" s="21">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="D82" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F82" s="21" t="s">
+        <v>297</v>
+      </c>
       <c r="G82" s="21"/>
-      <c r="H82" s="21"/>
+      <c r="H82" s="21" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="21"/>
-      <c r="D83" s="18"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="21"/>
-      <c r="H83" s="21"/>
+      <c r="B83" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="C83" s="21">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="D83" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="F83" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="G83" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="H83" s="21" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="21"/>
@@ -3629,7 +3703,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
@@ -3644,7 +3718,7 @@
         <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D5" t="s">
         <v>61</v>
@@ -3659,7 +3733,7 @@
         <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -3674,7 +3748,7 @@
         <v>67</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D7" t="s">
         <v>61</v>
@@ -3689,7 +3763,7 @@
         <v>68</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -3723,7 +3797,7 @@
         <v>132</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>60</v>
@@ -3753,7 +3827,7 @@
         <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D13" t="s">
         <v>60</v>
@@ -3913,7 +3987,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3987,10 +4061,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="36" t="s">
         <v>279</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>281</v>
       </c>
       <c r="D6" s="37"/>
     </row>
@@ -4000,7 +4074,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="37"/>
@@ -4011,7 +4085,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
@@ -4023,10 +4097,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4048,10 +4122,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>191</v>
+        <v>291</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>192</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4111,10 +4185,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4123,10 +4197,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>195</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,7 +4292,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C5" s="36" t="s">
         <v>136</v>
@@ -4232,7 +4306,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
@@ -4244,7 +4318,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
@@ -4256,7 +4330,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
@@ -4268,7 +4342,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
@@ -4516,7 +4590,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C30" s="36"/>
       <c r="D30" s="36"/>
@@ -4576,7 +4650,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>149</v>
@@ -4589,10 +4663,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D36" s="36"/>
     </row>
@@ -4602,10 +4676,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D37" s="36"/>
     </row>
@@ -4615,7 +4689,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C38" s="36"/>
       <c r="D38" s="36"/>
@@ -4735,7 +4809,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C48" s="36" t="s">
         <v>153</v>
@@ -4748,7 +4822,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C49" s="36"/>
       <c r="D49" s="36"/>
@@ -4770,10 +4844,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>204</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>206</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>208</v>
       </c>
       <c r="D51" s="36"/>
     </row>

</xml_diff>

<commit_message>
stop the dedicated offset codes. we can encode this into the operations
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="293">
   <si>
     <t>Name</t>
   </si>
@@ -942,72 +942,6 @@
   </si>
   <si>
     <t>Internal CPU register</t>
-  </si>
-  <si>
-    <t>SOFF1</t>
-  </si>
-  <si>
-    <t>SOFF2</t>
-  </si>
-  <si>
-    <t>SOFF12</t>
-  </si>
-  <si>
-    <t>Off1</t>
-  </si>
-  <si>
-    <t>Off2</t>
-  </si>
-  <si>
-    <t>R1OFFSET = Off1</t>
-  </si>
-  <si>
-    <t>R2OFFSET = Off2</t>
-  </si>
-  <si>
-    <t>R1OFFET = Off1; R2OFFSET = Off2</t>
-  </si>
-  <si>
-    <t>V8</t>
-  </si>
-  <si>
-    <t>V8V8</t>
-  </si>
-  <si>
-    <t>ROFF1</t>
-  </si>
-  <si>
-    <t>ROFF2</t>
-  </si>
-  <si>
-    <t>ROFF12</t>
-  </si>
-  <si>
-    <t>R1OFFSET = 0</t>
-  </si>
-  <si>
-    <t>R2OFFSET = 0</t>
-  </si>
-  <si>
-    <t>R1OFFET = 0; R2OFFSET = 0</t>
-  </si>
-  <si>
-    <t>OSOFF1</t>
-  </si>
-  <si>
-    <t>OSOFF2</t>
-  </si>
-  <si>
-    <t>OSOFF12</t>
-  </si>
-  <si>
-    <t>R1OFFSET = Off1; FLAG|S1RESET</t>
-  </si>
-  <si>
-    <t>R1OFFET = Off1; R2OFFSET = Off2; FLAG|S1RESET|S2RESET</t>
-  </si>
-  <si>
-    <t>R2OFFSET = Off2; FLAG|S1RESET|S2RESET</t>
   </si>
 </sst>
 </file>
@@ -1516,7 +1450,7 @@
   <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3523,217 +3457,93 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
-      <c r="B81" s="21" t="s">
-        <v>293</v>
-      </c>
-      <c r="C81" s="21">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="D81" s="18" t="str">
-        <f t="shared" si="4"/>
-        <v>4F</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="F81" s="21" t="s">
-        <v>296</v>
-      </c>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="21"/>
       <c r="G81" s="21"/>
-      <c r="H81" s="21" t="s">
-        <v>298</v>
-      </c>
+      <c r="H81" s="21"/>
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
-      <c r="B82" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="C82" s="21">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="D82" s="18" t="str">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="E82" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="F82" s="21" t="s">
-        <v>297</v>
-      </c>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="21"/>
       <c r="G82" s="21"/>
-      <c r="H82" s="21" t="s">
-        <v>299</v>
-      </c>
+      <c r="H82" s="21"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
-      <c r="B83" s="21" t="s">
-        <v>295</v>
-      </c>
-      <c r="C83" s="21">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="D83" s="18" t="str">
-        <f t="shared" si="4"/>
-        <v>51</v>
-      </c>
-      <c r="E83" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="F83" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="G83" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="H83" s="21" t="s">
-        <v>300</v>
-      </c>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
+      <c r="H83" s="21"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="21"/>
-      <c r="B84" s="21" t="s">
-        <v>303</v>
-      </c>
-      <c r="C84" s="21">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="D84" s="18" t="str">
-        <f t="shared" si="4"/>
-        <v>52</v>
-      </c>
-      <c r="E84" s="10" t="s">
-        <v>216</v>
-      </c>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="10"/>
       <c r="F84" s="21"/>
       <c r="G84" s="21"/>
-      <c r="H84" s="21" t="s">
-        <v>306</v>
-      </c>
+      <c r="H84" s="21"/>
     </row>
     <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="21"/>
-      <c r="B85" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="C85" s="21">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="D85" s="18" t="str">
-        <f t="shared" si="4"/>
-        <v>53</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>216</v>
-      </c>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="10"/>
       <c r="F85" s="21"/>
       <c r="G85" s="21"/>
-      <c r="H85" s="21" t="s">
-        <v>307</v>
-      </c>
+      <c r="H85" s="21"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="21"/>
-      <c r="B86" s="21" t="s">
-        <v>305</v>
-      </c>
-      <c r="C86" s="21">
-        <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="D86" s="18" t="str">
-        <f t="shared" si="4"/>
-        <v>54</v>
-      </c>
-      <c r="E86" s="10" t="s">
-        <v>216</v>
-      </c>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="10"/>
       <c r="F86" s="21"/>
       <c r="G86" s="21"/>
-      <c r="H86" s="21" t="s">
-        <v>308</v>
-      </c>
+      <c r="H86" s="21"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="21"/>
-      <c r="B87" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="C87" s="21">
-        <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="D87" s="18" t="str">
-        <f t="shared" ref="D87:D89" si="5">DEC2HEX(C87,2)</f>
-        <v>55</v>
-      </c>
-      <c r="E87" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="F87" s="21" t="s">
-        <v>296</v>
-      </c>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="21"/>
       <c r="G87" s="21"/>
-      <c r="H87" s="21" t="s">
-        <v>312</v>
-      </c>
+      <c r="H87" s="21"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="21"/>
-      <c r="B88" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="C88" s="21">
-        <f t="shared" ref="C88:C89" si="6">C87+1</f>
-        <v>86</v>
-      </c>
-      <c r="D88" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v>56</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="F88" s="21" t="s">
-        <v>297</v>
-      </c>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="21"/>
       <c r="G88" s="21"/>
-      <c r="H88" s="21" t="s">
-        <v>314</v>
-      </c>
+      <c r="H88" s="21"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="21"/>
-      <c r="B89" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="C89" s="21">
-        <f t="shared" si="6"/>
-        <v>87</v>
-      </c>
-      <c r="D89" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v>57</v>
-      </c>
-      <c r="E89" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="F89" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="G89" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="H89" s="21" t="s">
-        <v>313</v>
-      </c>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="21"/>
+      <c r="H89" s="21"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="21"/>
@@ -4995,6 +4805,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C12:C15"/>
     <mergeCell ref="D5:D41"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="D2:D4"/>
@@ -5011,7 +4822,6 @@
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C16:C20"/>
-    <mergeCell ref="C12:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
goodbye ENCRETN, hello #ALIGN
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="292">
   <si>
     <t>Name</t>
   </si>
@@ -678,9 +678,6 @@
   </si>
   <si>
     <t>ENCRETN</t>
-  </si>
-  <si>
-    <t>ENCON; RETN</t>
   </si>
   <si>
     <t>Turn on ROM encryption and return</t>
@@ -1449,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,7 +1463,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1478,13 +1475,13 @@
         <v>156</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -1505,7 +1502,7 @@
         <v>00</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -1514,13 +1511,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C3" s="2">
         <f>C2+1</f>
@@ -1531,7 +1528,7 @@
         <v>01</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
@@ -1540,13 +1537,13 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C4" s="21">
         <f>C3+1</f>
@@ -1557,7 +1554,7 @@
         <v>02</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -1566,13 +1563,13 @@
         <v>16</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C5" s="21">
         <f>C4+1</f>
@@ -1583,7 +1580,7 @@
         <v>03</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>17</v>
@@ -1592,7 +1589,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1608,13 +1605,13 @@
         <v>04</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1622,7 +1619,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" ref="C7:C87" si="1">C6+1</f>
+        <f t="shared" ref="C7:C80" si="1">C6+1</f>
         <v>5</v>
       </c>
       <c r="D7" s="18" t="str">
@@ -1630,7 +1627,7 @@
         <v>05</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F7" t="s">
         <v>28</v>
@@ -1642,7 +1639,7 @@
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
@@ -1653,19 +1650,19 @@
         <v>06</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
@@ -1676,13 +1673,13 @@
         <v>07</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1698,7 +1695,7 @@
         <v>08</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1717,7 +1714,7 @@
         <v>09</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -1726,7 +1723,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1742,7 +1739,7 @@
         <v>0A</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -1751,7 +1748,7 @@
         <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1767,7 +1764,7 @@
         <v>0B</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -1776,7 +1773,7 @@
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,7 +1789,7 @@
         <v>0C</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -1801,7 +1798,7 @@
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1817,7 +1814,7 @@
         <v>0D</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -1826,7 +1823,7 @@
         <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1842,7 +1839,7 @@
         <v>0E</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -1851,7 +1848,7 @@
         <v>16</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1867,7 +1864,7 @@
         <v>0F</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>17</v>
@@ -1876,12 +1873,12 @@
         <v>16</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
@@ -1892,7 +1889,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
@@ -1901,7 +1898,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1917,7 +1914,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>17</v>
@@ -1926,7 +1923,7 @@
         <v>16</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1942,7 +1939,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>17</v>
@@ -1951,7 +1948,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1970,7 +1967,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -1979,7 +1976,7 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1995,7 +1992,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
@@ -2004,7 +2001,7 @@
         <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2020,7 +2017,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -2029,7 +2026,7 @@
         <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2046,7 +2043,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
@@ -2055,7 +2052,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2074,7 +2071,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>17</v>
@@ -2083,7 +2080,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2102,7 +2099,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>17</v>
@@ -2111,7 +2108,7 @@
         <v>16</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2132,7 +2129,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>28</v>
@@ -2157,7 +2154,7 @@
         <v>1A</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>28</v>
@@ -2169,7 +2166,7 @@
     <row r="29" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C29" s="21">
         <f t="shared" si="1"/>
@@ -2180,7 +2177,7 @@
         <v>1B</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>28</v>
@@ -2189,13 +2186,13 @@
         <v>33</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
       <c r="B30" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C30" s="21">
         <f t="shared" si="1"/>
@@ -2206,7 +2203,7 @@
         <v>1C</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>28</v>
@@ -2228,7 +2225,7 @@
         <v>1D</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>28</v>
@@ -2242,7 +2239,7 @@
     </row>
     <row r="32" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C32" s="21">
         <f t="shared" si="1"/>
@@ -2253,7 +2250,7 @@
         <v>1E</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>28</v>
@@ -2262,7 +2259,7 @@
         <v>33</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2281,14 +2278,14 @@
         <v>1F</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J33" s="3"/>
     </row>
@@ -2306,7 +2303,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>28</v>
@@ -2330,7 +2327,7 @@
         <v>21</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>28</v>
@@ -2354,7 +2351,7 @@
         <v>22</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F36" s="21" t="s">
         <v>28</v>
@@ -2378,7 +2375,7 @@
         <v>23</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>28</v>
@@ -2401,7 +2398,7 @@
         <v>24</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F38" s="21" t="s">
         <v>28</v>
@@ -2422,7 +2419,7 @@
         <v>25</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>28</v>
@@ -2446,7 +2443,7 @@
         <v>26</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>28</v>
@@ -2455,7 +2452,7 @@
         <v>33</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2474,7 +2471,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>28</v>
@@ -2483,7 +2480,7 @@
         <v>33</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2502,7 +2499,7 @@
         <v>28</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>28</v>
@@ -2529,7 +2526,7 @@
         <v>29</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>28</v>
@@ -2553,7 +2550,7 @@
         <v>2A</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>28</v>
@@ -2577,7 +2574,7 @@
         <v>2B</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>28</v>
@@ -2601,7 +2598,7 @@
         <v>2C</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>28</v>
@@ -2625,7 +2622,7 @@
         <v>2D</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>28</v>
@@ -2649,7 +2646,7 @@
         <v>2E</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>28</v>
@@ -2673,7 +2670,7 @@
         <v>2F</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>28</v>
@@ -2682,7 +2679,7 @@
         <v>33</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="35"/>
@@ -2701,7 +2698,7 @@
         <v>30</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>28</v>
@@ -2710,7 +2707,7 @@
         <v>33</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="35"/>
@@ -2729,12 +2726,12 @@
         <v>31</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2755,14 +2752,14 @@
         <v>32</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F52" s="21" t="s">
         <v>28</v>
       </c>
       <c r="G52" s="21"/>
       <c r="H52" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2781,7 +2778,7 @@
         <v>33</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>28</v>
@@ -2790,7 +2787,7 @@
         <v>33</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2809,7 +2806,7 @@
         <v>34</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -2833,7 +2830,7 @@
         <v>35</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -2857,7 +2854,7 @@
         <v>36</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -2880,7 +2877,7 @@
         <v>37</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H57" s="14" t="s">
         <v>146</v>
@@ -2899,7 +2896,7 @@
         <v>38</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H58" s="14" t="s">
         <v>145</v>
@@ -2918,10 +2915,10 @@
         <v>39</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2937,48 +2934,55 @@
         <v>3A</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="21" t="s">
-        <v>204</v>
+      <c r="A61" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="C61" s="21">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="D61" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C61,2)</f>
         <v>3B</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="H61" s="21" t="s">
-        <v>205</v>
+        <v>257</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>282</v>
-      </c>
+      <c r="A62" s="12"/>
       <c r="B62" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C62" s="21">
+      <c r="C62" s="2">
         <f>C61+1</f>
         <v>60</v>
       </c>
       <c r="D62" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C62,2)</f>
         <v>3C</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>17</v>
@@ -2996,15 +3000,15 @@
         <v>249</v>
       </c>
       <c r="C63" s="2">
-        <f t="shared" si="1"/>
+        <f>C62+1</f>
         <v>61</v>
       </c>
       <c r="D63" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C63,2)</f>
         <v>3D</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>17</v>
@@ -3022,15 +3026,15 @@
         <v>250</v>
       </c>
       <c r="C64" s="2">
-        <f t="shared" si="1"/>
+        <f>C63+1</f>
         <v>62</v>
       </c>
       <c r="D64" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C64,2)</f>
         <v>3E</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>17</v>
@@ -3048,15 +3052,15 @@
         <v>251</v>
       </c>
       <c r="C65" s="2">
-        <f t="shared" si="1"/>
+        <f>C64+1</f>
         <v>63</v>
       </c>
       <c r="D65" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C65,2)</f>
         <v>3F</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>17</v>
@@ -3074,15 +3078,15 @@
         <v>252</v>
       </c>
       <c r="C66" s="2">
-        <f t="shared" si="1"/>
+        <f>C65+1</f>
         <v>64</v>
       </c>
       <c r="D66" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C66,2)</f>
         <v>40</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>17</v>
@@ -3090,7 +3094,7 @@
       <c r="G66" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="H66" s="5" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3100,15 +3104,15 @@
         <v>253</v>
       </c>
       <c r="C67" s="2">
-        <f t="shared" si="1"/>
+        <f>C66+1</f>
         <v>65</v>
       </c>
       <c r="D67" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C67,2)</f>
         <v>41</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>17</v>
@@ -3126,15 +3130,15 @@
         <v>254</v>
       </c>
       <c r="C68" s="2">
-        <f t="shared" si="1"/>
+        <f>C67+1</f>
         <v>66</v>
       </c>
       <c r="D68" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C68,2)</f>
         <v>42</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>17</v>
@@ -3152,15 +3156,15 @@
         <v>255</v>
       </c>
       <c r="C69" s="2">
-        <f t="shared" si="1"/>
+        <f>C68+1</f>
         <v>67</v>
       </c>
       <c r="D69" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C69,2)</f>
         <v>43</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>17</v>
@@ -3178,15 +3182,15 @@
         <v>256</v>
       </c>
       <c r="C70" s="2">
-        <f t="shared" si="1"/>
+        <f>C69+1</f>
         <v>68</v>
       </c>
       <c r="D70" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C70,2)</f>
         <v>44</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>17</v>
@@ -3199,20 +3203,22 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="2" t="s">
-        <v>257</v>
+      <c r="A71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" t="s">
+        <v>123</v>
       </c>
       <c r="C71" s="2">
-        <f t="shared" si="1"/>
+        <f>C70+1</f>
         <v>69</v>
       </c>
       <c r="D71" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C71,2)</f>
         <v>45</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>17</v>
@@ -3220,27 +3226,25 @@
       <c r="G71" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H71" s="5" t="s">
-        <v>231</v>
+      <c r="H71" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>122</v>
-      </c>
+      <c r="A72" s="12"/>
       <c r="B72" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C72" s="2">
-        <f t="shared" si="1"/>
+        <f>C71+1</f>
         <v>70</v>
       </c>
       <c r="D72" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C72,2)</f>
         <v>46</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>17</v>
@@ -3255,18 +3259,18 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="B73" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C73" s="2">
-        <f t="shared" si="1"/>
+        <f>C72+1</f>
         <v>71</v>
       </c>
       <c r="D73" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D73:D76" si="3">DEC2HEX(C73,2)</f>
         <v>47</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>17</v>
@@ -3281,18 +3285,18 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C74" s="2">
-        <f t="shared" si="1"/>
+        <f>C73+1</f>
         <v>72</v>
       </c>
       <c r="D74" s="18" t="str">
-        <f t="shared" ref="D74:D77" si="3">DEC2HEX(C74,2)</f>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>17</v>
@@ -3305,12 +3309,14 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
-      <c r="B75" t="s">
-        <v>126</v>
-      </c>
-      <c r="C75" s="2">
-        <f t="shared" si="1"/>
+      <c r="A75" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="B75" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="C75" s="21">
+        <f>C74+1</f>
         <v>73</v>
       </c>
       <c r="D75" s="18" t="str">
@@ -3318,27 +3324,25 @@
         <v>49</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="F75" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F75" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H75" s="2" t="s">
-        <v>225</v>
+      <c r="H75" s="21" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="21" t="s">
-        <v>283</v>
-      </c>
+      <c r="A76" s="12"/>
       <c r="B76" s="21" t="s">
         <v>284</v>
       </c>
       <c r="C76" s="21">
-        <f t="shared" si="1"/>
+        <f>C75+1</f>
         <v>74</v>
       </c>
       <c r="D76" s="18" t="str">
@@ -3346,7 +3350,7 @@
         <v>4A</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F76" s="21" t="s">
         <v>17</v>
@@ -3361,18 +3365,18 @@
     <row r="77" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="B77" s="21" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C77" s="21">
-        <f t="shared" si="1"/>
+        <f>C76+1</f>
         <v>75</v>
       </c>
       <c r="D77" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D77:D79" si="4">DEC2HEX(C77,2)</f>
         <v>4B</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F77" s="21" t="s">
         <v>17</v>
@@ -3387,18 +3391,18 @@
     <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="B78" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C78" s="21">
-        <f t="shared" si="1"/>
+        <f>C77+1</f>
         <v>76</v>
       </c>
       <c r="D78" s="18" t="str">
-        <f t="shared" ref="D78:D86" si="4">DEC2HEX(C78,2)</f>
+        <f t="shared" si="4"/>
         <v>4C</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F78" s="21" t="s">
         <v>17</v>
@@ -3411,12 +3415,14 @@
       </c>
     </row>
     <row r="79" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
-      <c r="B79" s="21" t="s">
-        <v>286</v>
+      <c r="A79" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="B79" s="32" t="s">
+        <v>275</v>
       </c>
       <c r="C79" s="21">
-        <f t="shared" si="1"/>
+        <f>C78+1</f>
         <v>77</v>
       </c>
       <c r="D79" s="18" t="str">
@@ -3426,34 +3432,19 @@
       <c r="E79" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="F79" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G79" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H79" s="21" t="s">
-        <v>225</v>
-      </c>
+      <c r="F79"/>
+      <c r="G79"/>
+      <c r="H79"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="32" t="s">
-        <v>290</v>
-      </c>
-      <c r="B80" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="C80" s="21">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="D80" s="18" t="str">
-        <f t="shared" si="4"/>
-        <v>4E</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>216</v>
-      </c>
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="21"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
@@ -3465,16 +3456,7 @@
       <c r="G81" s="21"/>
       <c r="H81" s="21"/>
     </row>
-    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="21"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="21"/>
-      <c r="H82" s="21"/>
-    </row>
+    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
       <c r="B83" s="21"/>
@@ -3629,7 +3611,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
@@ -3644,7 +3626,7 @@
         <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D5" t="s">
         <v>61</v>
@@ -3659,7 +3641,7 @@
         <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -3674,7 +3656,7 @@
         <v>67</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" t="s">
         <v>61</v>
@@ -3689,7 +3671,7 @@
         <v>68</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -3723,7 +3705,7 @@
         <v>132</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>60</v>
@@ -3753,7 +3735,7 @@
         <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D13" t="s">
         <v>60</v>
@@ -3987,10 +3969,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D6" s="37"/>
     </row>
@@ -4000,7 +3982,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="37"/>
@@ -4011,7 +3993,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
@@ -4023,10 +4005,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>244</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4048,10 +4030,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>291</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,7 +4200,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C5" s="36" t="s">
         <v>136</v>
@@ -4232,7 +4214,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
@@ -4244,7 +4226,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
@@ -4256,7 +4238,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
@@ -4268,7 +4250,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
@@ -4735,7 +4717,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C48" s="36" t="s">
         <v>153</v>
@@ -4748,7 +4730,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C49" s="36"/>
       <c r="D49" s="36"/>
@@ -4773,7 +4755,7 @@
         <v>204</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D51" s="36"/>
     </row>
@@ -4805,11 +4787,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D5:D41"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C39:C40"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="D42:D51"/>
     <mergeCell ref="C48:C50"/>
@@ -4822,6 +4799,11 @@
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C16:C20"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D5:D41"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C39:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
move ROM to addr 0 instead of end
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doridian\Documents\Visual Studio 2017\Projects\HMCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{33FF842C-741A-4A61-8579-C33D75B062FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B4D44E95-7F78-42E4-9F84-BF0779A742C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="315">
   <si>
     <t>Name</t>
   </si>
@@ -287,15 +287,9 @@
     <t>0x0000</t>
   </si>
   <si>
-    <t>ROMBASE</t>
-  </si>
-  <si>
     <t>User memory</t>
   </si>
   <si>
-    <t>512 bytes</t>
-  </si>
-  <si>
     <t>Interrupt Handlers (inc IHBASE)</t>
   </si>
   <si>
@@ -303,9 +297,6 @@
   </si>
   <si>
     <t>Remaining memory</t>
-  </si>
-  <si>
-    <t>ROM size (Variable!)</t>
   </si>
   <si>
     <t>General purpose registers</t>
@@ -1001,6 +992,12 @@
   </si>
   <si>
     <t>Bootloader key</t>
+  </si>
+  <si>
+    <t>ROMEND</t>
+  </si>
+  <si>
+    <t>1024 bytes</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1104,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1179,6 +1176,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1499,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,7 +1516,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1525,16 +1525,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E1" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -1555,7 +1555,7 @@
         <v>00</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -1564,13 +1564,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C3" s="2">
         <f>C2+1</f>
@@ -1581,7 +1581,7 @@
         <v>01</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
@@ -1590,13 +1590,13 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C4" s="20">
         <f>C3+1</f>
@@ -1607,7 +1607,7 @@
         <v>02</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -1616,13 +1616,13 @@
         <v>16</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
       <c r="B5" s="31" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" s="20">
         <f>C4+1</f>
@@ -1633,7 +1633,7 @@
         <v>03</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>17</v>
@@ -1642,7 +1642,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1658,13 +1658,13 @@
         <v>04</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1680,19 +1680,19 @@
         <v>05</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F7" t="s">
         <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
@@ -1703,19 +1703,19 @@
         <v>06</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
@@ -1726,13 +1726,13 @@
         <v>07</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1748,7 +1748,7 @@
         <v>08</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1767,7 +1767,7 @@
         <v>09</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -1776,7 +1776,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
         <v>0A</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -1801,7 +1801,7 @@
         <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
         <v>0B</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -1826,7 +1826,7 @@
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1842,7 +1842,7 @@
         <v>0C</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -1851,7 +1851,7 @@
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1867,7 +1867,7 @@
         <v>0D</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -1876,7 +1876,7 @@
         <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1892,7 +1892,7 @@
         <v>0E</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -1901,12 +1901,12 @@
         <v>16</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
@@ -1917,7 +1917,7 @@
         <v>0F</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>17</v>
@@ -1926,12 +1926,12 @@
         <v>16</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
@@ -1942,7 +1942,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
@@ -1951,12 +1951,12 @@
         <v>16</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="1"/>
@@ -1967,7 +1967,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>17</v>
@@ -1976,12 +1976,12 @@
         <v>16</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="1"/>
@@ -1992,7 +1992,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>17</v>
@@ -2001,7 +2001,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2020,7 +2020,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -2029,7 +2029,7 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
@@ -2054,7 +2054,7 @@
         <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2070,7 +2070,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -2079,7 +2079,7 @@
         <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2096,7 +2096,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
@@ -2105,7 +2105,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2124,7 +2124,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>17</v>
@@ -2133,7 +2133,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2152,7 +2152,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>17</v>
@@ -2161,17 +2161,17 @@
         <v>16</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C27" s="20">
         <f t="shared" si="1"/>
@@ -2182,7 +2182,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>28</v>
@@ -2191,12 +2191,12 @@
         <v>33</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C28" s="20">
         <f t="shared" si="1"/>
@@ -2207,7 +2207,7 @@
         <v>1A</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>28</v>
@@ -2219,7 +2219,7 @@
     <row r="29" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="20" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C29" s="20">
         <f t="shared" si="1"/>
@@ -2230,7 +2230,7 @@
         <v>1B</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>28</v>
@@ -2239,13 +2239,13 @@
         <v>33</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
       <c r="B30" s="20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C30" s="20">
         <f t="shared" si="1"/>
@@ -2256,7 +2256,7 @@
         <v>1C</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>28</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="31" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C31" s="20">
         <f t="shared" si="1"/>
@@ -2278,7 +2278,7 @@
         <v>1D</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F31" s="20" t="s">
         <v>28</v>
@@ -2287,12 +2287,12 @@
         <v>33</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C32" s="20">
         <f t="shared" si="1"/>
@@ -2303,7 +2303,7 @@
         <v>1E</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F32" s="20" t="s">
         <v>28</v>
@@ -2312,7 +2312,7 @@
         <v>33</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2331,21 +2331,21 @@
         <v>1F</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F33" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J33" s="3"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="1"/>
@@ -2356,7 +2356,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>28</v>
@@ -2369,7 +2369,7 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" si="1"/>
@@ -2380,7 +2380,7 @@
         <v>21</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>28</v>
@@ -2404,7 +2404,7 @@
         <v>22</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F36" s="20" t="s">
         <v>28</v>
@@ -2428,7 +2428,7 @@
         <v>23</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>28</v>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="38" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C38" s="20">
         <f t="shared" si="1"/>
@@ -2451,7 +2451,7 @@
         <v>24</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>28</v>
@@ -2461,7 +2461,7 @@
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C39" s="20">
         <f t="shared" si="1"/>
@@ -2472,7 +2472,7 @@
         <v>25</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>28</v>
@@ -2496,7 +2496,7 @@
         <v>26</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>28</v>
@@ -2505,7 +2505,7 @@
         <v>33</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2524,7 +2524,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>28</v>
@@ -2533,7 +2533,7 @@
         <v>33</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2552,7 +2552,7 @@
         <v>28</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F42" s="20" t="s">
         <v>28</v>
@@ -2562,13 +2562,13 @@
         <v>36</v>
       </c>
       <c r="J42" s="34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C43" s="2">
         <f t="shared" si="1"/>
@@ -2579,7 +2579,7 @@
         <v>29</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>28</v>
@@ -2592,7 +2592,7 @@
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C44" s="2">
         <f t="shared" si="1"/>
@@ -2603,7 +2603,7 @@
         <v>2A</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>28</v>
@@ -2627,7 +2627,7 @@
         <v>2B</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F45" s="20" t="s">
         <v>28</v>
@@ -2651,7 +2651,7 @@
         <v>2C</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F46" s="20" t="s">
         <v>28</v>
@@ -2664,7 +2664,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C47" s="2">
         <f t="shared" si="1"/>
@@ -2675,7 +2675,7 @@
         <v>2D</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>28</v>
@@ -2688,7 +2688,7 @@
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" si="1"/>
@@ -2699,7 +2699,7 @@
         <v>2E</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>28</v>
@@ -2723,7 +2723,7 @@
         <v>2F</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>28</v>
@@ -2732,7 +2732,7 @@
         <v>33</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="34"/>
@@ -2751,7 +2751,7 @@
         <v>30</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>28</v>
@@ -2760,7 +2760,7 @@
         <v>33</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="34"/>
@@ -2779,12 +2779,12 @@
         <v>31</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2805,14 +2805,14 @@
         <v>32</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F52" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G52" s="20"/>
       <c r="H52" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2831,7 +2831,7 @@
         <v>33</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F53" s="20" t="s">
         <v>28</v>
@@ -2840,7 +2840,7 @@
         <v>33</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2859,7 +2859,7 @@
         <v>34</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -2883,7 +2883,7 @@
         <v>35</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -2907,7 +2907,7 @@
         <v>36</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -2919,7 +2919,7 @@
     </row>
     <row r="57" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C57" s="13">
         <f t="shared" si="1"/>
@@ -2930,15 +2930,15 @@
         <v>37</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C58" s="13">
         <f t="shared" si="1"/>
@@ -2949,15 +2949,15 @@
         <v>38</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C59" s="15">
         <f t="shared" si="1"/>
@@ -2968,15 +2968,15 @@
         <v>39</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C60" s="15">
         <f t="shared" si="1"/>
@@ -2987,18 +2987,18 @@
         <v>3A</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C61" s="20">
         <f t="shared" si="1"/>
@@ -3009,7 +3009,7 @@
         <v>3B</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>17</v>
@@ -3018,13 +3018,13 @@
         <v>16</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C62" s="2">
         <f t="shared" ref="C62:C79" si="4">C61+1</f>
@@ -3035,7 +3035,7 @@
         <v>3C</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>17</v>
@@ -3044,13 +3044,13 @@
         <v>16</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C63" s="2">
         <f t="shared" si="4"/>
@@ -3061,7 +3061,7 @@
         <v>3D</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>17</v>
@@ -3070,13 +3070,13 @@
         <v>16</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C64" s="2">
         <f t="shared" si="4"/>
@@ -3087,7 +3087,7 @@
         <v>3E</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>17</v>
@@ -3096,13 +3096,13 @@
         <v>16</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C65" s="2">
         <f t="shared" si="4"/>
@@ -3113,7 +3113,7 @@
         <v>3F</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>17</v>
@@ -3122,13 +3122,13 @@
         <v>16</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C66" s="2">
         <f t="shared" si="4"/>
@@ -3139,7 +3139,7 @@
         <v>40</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>17</v>
@@ -3148,13 +3148,13 @@
         <v>16</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C67" s="2">
         <f t="shared" si="4"/>
@@ -3165,7 +3165,7 @@
         <v>41</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>17</v>
@@ -3174,13 +3174,13 @@
         <v>16</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C68" s="2">
         <f t="shared" si="4"/>
@@ -3191,7 +3191,7 @@
         <v>42</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>17</v>
@@ -3200,13 +3200,13 @@
         <v>16</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C69" s="2">
         <f t="shared" si="4"/>
@@ -3217,7 +3217,7 @@
         <v>43</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>17</v>
@@ -3226,13 +3226,13 @@
         <v>16</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C70" s="2">
         <f t="shared" si="4"/>
@@ -3243,7 +3243,7 @@
         <v>44</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>17</v>
@@ -3252,15 +3252,15 @@
         <v>16</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B71" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C71" s="2">
         <f t="shared" si="4"/>
@@ -3271,7 +3271,7 @@
         <v>45</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>17</v>
@@ -3280,13 +3280,13 @@
         <v>16</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C72" s="2">
         <f t="shared" si="4"/>
@@ -3297,7 +3297,7 @@
         <v>46</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>17</v>
@@ -3306,13 +3306,13 @@
         <v>16</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C73" s="2">
         <f t="shared" si="4"/>
@@ -3323,7 +3323,7 @@
         <v>47</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>17</v>
@@ -3332,13 +3332,13 @@
         <v>16</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C74" s="2">
         <f t="shared" si="4"/>
@@ -3349,7 +3349,7 @@
         <v>48</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>17</v>
@@ -3358,15 +3358,15 @@
         <v>16</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C75" s="20">
         <f t="shared" si="4"/>
@@ -3377,7 +3377,7 @@
         <v>49</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F75" s="20" t="s">
         <v>17</v>
@@ -3386,13 +3386,13 @@
         <v>16</v>
       </c>
       <c r="H75" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="20" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C76" s="20">
         <f t="shared" si="4"/>
@@ -3403,7 +3403,7 @@
         <v>4A</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F76" s="20" t="s">
         <v>17</v>
@@ -3412,13 +3412,13 @@
         <v>16</v>
       </c>
       <c r="H76" s="20" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="20" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C77" s="20">
         <f t="shared" si="4"/>
@@ -3429,7 +3429,7 @@
         <v>4B</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F77" s="20" t="s">
         <v>17</v>
@@ -3438,13 +3438,13 @@
         <v>16</v>
       </c>
       <c r="H77" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="20" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C78" s="20">
         <f t="shared" si="4"/>
@@ -3455,7 +3455,7 @@
         <v>4C</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F78" s="20" t="s">
         <v>17</v>
@@ -3464,15 +3464,15 @@
         <v>16</v>
       </c>
       <c r="H78" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C79" s="20">
         <f t="shared" si="4"/>
@@ -3483,7 +3483,7 @@
         <v>4D</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F79"/>
       <c r="G79"/>
@@ -3664,7 +3664,7 @@
         <v>63</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>
@@ -3679,7 +3679,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -3694,7 +3694,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D6" t="s">
         <v>60</v>
@@ -3709,7 +3709,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D7" t="s">
         <v>60</v>
@@ -3724,7 +3724,7 @@
         <v>67</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D8" t="s">
         <v>60</v>
@@ -3755,10 +3755,10 @@
         <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>59</v>
@@ -3773,7 +3773,7 @@
         <v>52</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D12" t="s">
         <v>59</v>
@@ -3788,7 +3788,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D13" t="s">
         <v>59</v>
@@ -3831,22 +3831,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>143</v>
-      </c>
       <c r="F1" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3854,17 +3854,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G2" s="21"/>
       <c r="I2" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3873,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="21"/>
@@ -3881,7 +3881,7 @@
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="I3" s="25" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3890,7 +3890,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="21"/>
@@ -3898,7 +3898,7 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="I4" s="26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3907,18 +3907,18 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3927,13 +3927,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G6" s="21"/>
     </row>
@@ -3975,10 +3975,10 @@
         <v>21</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4001,7 +4001,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D4" s="36"/>
     </row>
@@ -4022,10 +4022,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D6" s="36"/>
     </row>
@@ -4035,7 +4035,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="36"/>
@@ -4046,10 +4046,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4058,10 +4058,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4083,10 +4083,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4095,13 +4095,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4110,7 +4110,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="35"/>
       <c r="D13" s="32"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4146,10 +4146,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" t="s">
         <v>160</v>
-      </c>
-      <c r="D16" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4158,10 +4158,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4187,8 +4187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60:D81"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4211,7 +4211,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4219,13 +4219,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4234,13 +4234,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4249,10 +4249,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D4" s="35"/>
     </row>
@@ -4262,7 +4262,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -4274,10 +4274,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="20"/>
@@ -4288,7 +4288,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="35"/>
@@ -4300,7 +4300,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
@@ -4312,7 +4312,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
@@ -4324,7 +4324,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
@@ -4335,7 +4335,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
@@ -4355,7 +4355,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="35"/>
@@ -4369,7 +4369,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D14" s="35"/>
     </row>
@@ -4379,7 +4379,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C15" s="36"/>
       <c r="D15" s="35"/>
@@ -4390,7 +4390,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C16" s="36"/>
       <c r="D16" s="35"/>
@@ -4401,10 +4401,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D17" s="35"/>
     </row>
@@ -4414,7 +4414,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
@@ -4434,7 +4434,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
@@ -4445,7 +4445,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
@@ -4456,7 +4456,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
@@ -4467,7 +4467,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="35"/>
@@ -4489,7 +4489,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="35"/>
@@ -4509,7 +4509,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C27" s="37"/>
       <c r="D27" s="35"/>
@@ -4523,7 +4523,7 @@
         <v>73</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D28" s="35"/>
     </row>
@@ -4533,7 +4533,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C29" s="35"/>
       <c r="D29" s="35"/>
@@ -4544,7 +4544,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C30" s="35" t="s">
         <v>75</v>
@@ -4557,7 +4557,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
@@ -4568,7 +4568,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="35"/>
@@ -4579,7 +4579,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C33" s="35" t="s">
         <v>74</v>
@@ -4592,7 +4592,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C34" s="35"/>
       <c r="D34" s="35"/>
@@ -4616,7 +4616,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C36" s="35"/>
       <c r="D36" s="35"/>
@@ -4635,7 +4635,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C38" s="35" t="s">
         <v>79</v>
@@ -4648,7 +4648,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C39" s="35"/>
       <c r="D39" s="35"/>
@@ -4660,7 +4660,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C40" s="35"/>
       <c r="D40" s="35"/>
@@ -4681,10 +4681,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D42" s="35"/>
       <c r="E42" s="33"/>
@@ -4704,10 +4704,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D44" s="35"/>
     </row>
@@ -4717,10 +4717,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D45" s="35"/>
     </row>
@@ -4730,10 +4730,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C46" s="35" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D46" s="35"/>
     </row>
@@ -4743,7 +4743,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C47" s="35"/>
       <c r="D47" s="35"/>
@@ -4762,10 +4762,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C49" s="35" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D49" s="35"/>
     </row>
@@ -4775,7 +4775,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C50" s="35"/>
       <c r="D50" s="35"/>
@@ -4786,7 +4786,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C51" s="35"/>
       <c r="D51" s="35"/>
@@ -4797,7 +4797,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C52" s="35"/>
       <c r="D52" s="35"/>
@@ -4817,7 +4817,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C54" s="35" t="s">
         <v>80</v>
@@ -4830,7 +4830,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C55" s="35"/>
       <c r="D55" s="35"/>
@@ -4841,7 +4841,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C56" s="35"/>
       <c r="D56" s="35"/>
@@ -4852,7 +4852,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C57" s="35"/>
       <c r="D57" s="35"/>
@@ -4863,7 +4863,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C58" s="35"/>
       <c r="D58" s="35"/>
@@ -4883,13 +4883,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D60" s="35" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -4898,7 +4898,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C61" s="35"/>
       <c r="D61" s="35"/>
@@ -4909,10 +4909,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C62" s="33" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D62" s="35"/>
     </row>
@@ -4922,10 +4922,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D63" s="35"/>
     </row>
@@ -4935,7 +4935,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C64" s="35"/>
       <c r="D64" s="35"/>
@@ -4946,10 +4946,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D65" s="35"/>
     </row>
@@ -4959,7 +4959,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C66" s="35"/>
       <c r="D66" s="35"/>
@@ -4970,7 +4970,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C67" s="35"/>
       <c r="D67" s="35"/>
@@ -4981,7 +4981,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C68" s="35"/>
       <c r="D68" s="35"/>
@@ -4992,7 +4992,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C69" s="35"/>
       <c r="D69" s="35"/>
@@ -5003,7 +5003,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C70" s="35"/>
       <c r="D70" s="35"/>
@@ -5014,7 +5014,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C71" s="35"/>
       <c r="D71" s="35"/>
@@ -5025,7 +5025,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C72" s="35"/>
       <c r="D72" s="35"/>
@@ -5036,7 +5036,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C73" s="35"/>
       <c r="D73" s="35"/>
@@ -5047,10 +5047,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C74" s="35" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D74" s="35"/>
     </row>
@@ -5060,7 +5060,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C75" s="35"/>
       <c r="D75" s="35"/>
@@ -5082,10 +5082,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="20" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C77" s="35" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D77" s="35"/>
     </row>
@@ -5095,7 +5095,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C78" s="35"/>
       <c r="D78" s="35"/>
@@ -5106,7 +5106,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="20" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C79" s="35"/>
       <c r="D79" s="35"/>
@@ -5117,7 +5117,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C80" s="35"/>
       <c r="D80" s="35"/>
@@ -5128,7 +5128,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="20" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C81" s="35"/>
       <c r="D81" s="35"/>
@@ -5143,16 +5143,20 @@
       </c>
       <c r="C82" s="35"/>
       <c r="D82" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C83" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C33:C36"/>
     <mergeCell ref="D3:D59"/>
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="C63:C64"/>
@@ -5169,10 +5173,6 @@
     <mergeCell ref="C17:C25"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="C33:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5183,8 +5183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5203,53 +5203,53 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>86</v>
+      <c r="A2" s="38" t="s">
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>82</v>
+      <c r="A3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>88</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="7"/>
+        <v>82</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>246</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>85</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
actually CALL user interrupts
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doridian\Documents\Visual Studio 2017\Projects\HMCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{90E96F52-2D44-438C-8F89-7A3BA0F7D007}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{42A4A329-2AAF-420D-9EAF-B75F66DEC3FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="323">
   <si>
     <t>Name</t>
   </si>
@@ -140,9 +140,6 @@
     <t>JNE</t>
   </si>
   <si>
-    <t>PC = Const | Reg</t>
-  </si>
-  <si>
     <t>CALL</t>
   </si>
   <si>
@@ -326,35 +323,6 @@
     <t>DIVF</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Those all </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PUSH PC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> when they jump (after setting PC)</t>
-    </r>
-  </si>
-  <si>
-    <t>SP -= 4, Reg = RAM[SP]</t>
-  </si>
-  <si>
     <t>ENCREG1</t>
   </si>
   <si>
@@ -388,12 +356,6 @@
     <t>ENCOFF</t>
   </si>
   <si>
-    <t>Encryption = On</t>
-  </si>
-  <si>
-    <t>Encryption = Off</t>
-  </si>
-  <si>
     <t>Load ROM encryption key</t>
   </si>
   <si>
@@ -469,12 +431,6 @@
     <t>(Re)SetPos</t>
   </si>
   <si>
-    <t>2M</t>
-  </si>
-  <si>
-    <t>eRAM</t>
-  </si>
-  <si>
     <t>ENCREG12</t>
   </si>
   <si>
@@ -562,9 +518,6 @@
     <t>RegDst = RegSrc</t>
   </si>
   <si>
-    <t>RAM[SP] = Reg, SP += 4</t>
-  </si>
-  <si>
     <t>RegDst +=  RegSrc</t>
   </si>
   <si>
@@ -613,12 +566,6 @@
     <t>RegDst &amp;= !(RegSrc)</t>
   </si>
   <si>
-    <t>Reg == 0 -&gt; PC = Reg2</t>
-  </si>
-  <si>
-    <t>Reg != 0 -&gt; PC = Reg2</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -688,15 +635,6 @@
     <t>POP64</t>
   </si>
   <si>
-    <t>RAM[SP] = Reg, SP += 8</t>
-  </si>
-  <si>
-    <t>SP -= 8, Reg = RAM[SP]</t>
-  </si>
-  <si>
-    <t>SP -= 4, PC = RAM[SP]</t>
-  </si>
-  <si>
     <t>CALL RAM[IHBASE+Reg*4]</t>
   </si>
   <si>
@@ -757,21 +695,12 @@
     <t>MUL64F</t>
   </si>
   <si>
-    <t>PUSH64 $R12; PUSH64 $R34; PUSH64 R56</t>
-  </si>
-  <si>
-    <t>POP64 R56; POP64 $R34; POP64 $R12</t>
-  </si>
-  <si>
     <t>Extra</t>
   </si>
   <si>
     <t>MSR</t>
   </si>
   <si>
-    <t>Internal CPU register</t>
-  </si>
-  <si>
     <t>BSP</t>
   </si>
   <si>
@@ -1007,6 +936,69 @@
   </si>
   <si>
     <t>Bootloader is loaded here, but can be overwritten later</t>
+  </si>
+  <si>
+    <t>CSP -= 4, RAM[SP] = Reg</t>
+  </si>
+  <si>
+    <t>Reg = RAM[SP], CSP += 4</t>
+  </si>
+  <si>
+    <t>CSP -= 8, RAM[SP] = Reg</t>
+  </si>
+  <si>
+    <t>Reg = RAM[SP], CSP += 8</t>
+  </si>
+  <si>
+    <t>CSP = BSP, BSP = POP, PC = POP</t>
+  </si>
+  <si>
+    <t>PUSH64 R12; PUSH64 R34; PUSH64 R56</t>
+  </si>
+  <si>
+    <t>POP64 R56; POP64 R34; POP64 R12</t>
+  </si>
+  <si>
+    <t>PUSH PC, PUSH BSP, BSP = CSP, JMP Reg</t>
+  </si>
+  <si>
+    <t>Internal CPU register (contains FLAGR [8 bit])</t>
+  </si>
+  <si>
+    <t>FLAGR &amp;= ~FLAG_ENCON</t>
+  </si>
+  <si>
+    <t>FLAGR |= FLAG_ENCON</t>
+  </si>
+  <si>
+    <t>Unset all CMP from FLAGR. Set FLAG_EQ and FLAG_LT appropriately</t>
+  </si>
+  <si>
+    <t>Check if !FLAG_LT or FLAG_EQ</t>
+  </si>
+  <si>
+    <t>Check if FLAG_LT or FLAG_EQ</t>
+  </si>
+  <si>
+    <t>RegCheck</t>
+  </si>
+  <si>
+    <t>Check if RegCheck = 0</t>
+  </si>
+  <si>
+    <t>Check if RegCheck != 0</t>
+  </si>
+  <si>
+    <t>Check if FLAG_EQ</t>
+  </si>
+  <si>
+    <t>Check if !FLAG_EQ</t>
+  </si>
+  <si>
+    <t>Check if !FLAG_LT</t>
+  </si>
+  <si>
+    <t>Check if FLAG_LT</t>
   </si>
 </sst>
 </file>
@@ -1178,9 +1170,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1191,6 +1180,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1511,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,13 +1514,13 @@
     <col min="5" max="5" width="9.140625" style="20"/>
     <col min="6" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="59.7109375" customWidth="1"/>
-    <col min="9" max="9" width="38.85546875" customWidth="1"/>
+    <col min="9" max="9" width="61.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1537,16 +1529,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
@@ -1567,7 +1559,7 @@
         <v>00</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -1576,13 +1568,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C3" s="2">
         <f>C2+1</f>
@@ -1593,7 +1585,7 @@
         <v>01</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
@@ -1602,13 +1594,13 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C4" s="20">
         <f>C3+1</f>
@@ -1619,7 +1611,7 @@
         <v>02</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -1628,13 +1620,13 @@
         <v>16</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
       <c r="B5" s="31" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="C5" s="20">
         <f>C4+1</f>
@@ -1645,7 +1637,7 @@
         <v>03</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>17</v>
@@ -1654,7 +1646,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1670,13 +1662,13 @@
         <v>04</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>169</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1692,19 +1684,19 @@
         <v>05</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F7" t="s">
         <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
@@ -1715,19 +1707,19 @@
         <v>06</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>211</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
@@ -1738,13 +1730,13 @@
         <v>07</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>212</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1760,12 +1752,12 @@
         <v>08</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -1779,7 +1771,7 @@
         <v>09</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -1788,7 +1780,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1804,7 +1796,7 @@
         <v>0A</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -1813,7 +1805,7 @@
         <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1829,7 +1821,7 @@
         <v>0B</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -1838,7 +1830,7 @@
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1854,7 +1846,7 @@
         <v>0C</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -1863,7 +1855,7 @@
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1879,7 +1871,7 @@
         <v>0D</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -1888,12 +1880,12 @@
         <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="1"/>
@@ -1904,7 +1896,7 @@
         <v>0E</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -1913,12 +1905,12 @@
         <v>16</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
@@ -1929,7 +1921,7 @@
         <v>0F</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>17</v>
@@ -1938,12 +1930,12 @@
         <v>16</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
@@ -1954,7 +1946,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
@@ -1963,12 +1955,12 @@
         <v>16</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="1"/>
@@ -1979,7 +1971,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>17</v>
@@ -1988,12 +1980,12 @@
         <v>16</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="1"/>
@@ -2004,7 +1996,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>17</v>
@@ -2013,7 +2005,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2032,7 +2024,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -2041,7 +2033,7 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2057,7 +2049,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
@@ -2066,7 +2058,7 @@
         <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2082,7 +2074,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -2091,7 +2083,7 @@
         <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2108,7 +2100,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
@@ -2117,7 +2109,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2136,7 +2128,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>17</v>
@@ -2145,7 +2137,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2164,7 +2156,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>17</v>
@@ -2173,17 +2165,17 @@
         <v>16</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C27" s="20">
         <f t="shared" si="1"/>
@@ -2194,7 +2186,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>28</v>
@@ -2202,13 +2194,16 @@
       <c r="G27" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="20" t="s">
-        <v>150</v>
+      <c r="H27" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="I27" s="35" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C28" s="20">
         <f t="shared" si="1"/>
@@ -2219,7 +2214,7 @@
         <v>1A</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>28</v>
@@ -2227,11 +2222,13 @@
       <c r="G28" s="20" t="s">
         <v>33</v>
       </c>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
     </row>
     <row r="29" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="20" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C29" s="20">
         <f t="shared" si="1"/>
@@ -2242,7 +2239,7 @@
         <v>1B</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>28</v>
@@ -2250,14 +2247,15 @@
       <c r="G29" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H29" s="20" t="s">
-        <v>207</v>
-      </c>
+      <c r="H29" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="I29" s="35"/>
     </row>
     <row r="30" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
       <c r="B30" s="20" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C30" s="20">
         <f t="shared" si="1"/>
@@ -2268,7 +2266,7 @@
         <v>1C</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>28</v>
@@ -2276,10 +2274,12 @@
       <c r="G30" s="20" t="s">
         <v>33</v>
       </c>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
     </row>
     <row r="31" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C31" s="20">
         <f t="shared" si="1"/>
@@ -2290,7 +2290,7 @@
         <v>1D</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F31" s="20" t="s">
         <v>28</v>
@@ -2299,12 +2299,13 @@
         <v>33</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>152</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="20" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="C32" s="20">
         <f t="shared" si="1"/>
@@ -2315,7 +2316,7 @@
         <v>1E</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F32" s="20" t="s">
         <v>28</v>
@@ -2324,8 +2325,9 @@
         <v>33</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>227</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="I32" s="35"/>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -2343,21 +2345,21 @@
         <v>1F</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F33" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G33" s="20"/>
-      <c r="H33" s="2" t="s">
-        <v>167</v>
+      <c r="H33" s="35" t="s">
+        <v>160</v>
       </c>
       <c r="J33" s="3"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="1"/>
@@ -2368,20 +2370,22 @@
         <v>20</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="4"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="4" t="s">
+        <v>314</v>
+      </c>
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" si="1"/>
@@ -2392,14 +2396,16 @@
         <v>21</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="4"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="4" t="s">
+        <v>315</v>
+      </c>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2416,14 +2422,16 @@
         <v>22</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F36" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="4"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="4" t="s">
+        <v>319</v>
+      </c>
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2440,19 +2448,21 @@
         <v>23</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="4"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="4" t="s">
+        <v>320</v>
+      </c>
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="20" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C38" s="20">
         <f t="shared" si="1"/>
@@ -2463,17 +2473,20 @@
         <v>24</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I38" s="4"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="4" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C39" s="20">
         <f t="shared" si="1"/>
@@ -2484,14 +2497,16 @@
         <v>25</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="4" t="s">
+        <v>322</v>
+      </c>
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2508,18 +2523,18 @@
         <v>26</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F40" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G40" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="I40" s="2"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="4" t="s">
+        <v>317</v>
+      </c>
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2536,24 +2551,24 @@
         <v>27</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F41" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="G41" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G41" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I41" s="2"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="4" t="s">
+        <v>318</v>
+      </c>
       <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42" s="2">
         <f t="shared" si="1"/>
@@ -2564,23 +2579,20 @@
         <v>28</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F42" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G42" s="20"/>
-      <c r="H42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J42" s="35" t="s">
-        <v>98</v>
+      <c r="H42" s="39" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C43" s="2">
         <f t="shared" si="1"/>
@@ -2591,20 +2603,21 @@
         <v>29</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="4" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C44" s="2">
         <f t="shared" si="1"/>
@@ -2615,20 +2628,21 @@
         <v>2A</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="4" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C45" s="2">
         <f t="shared" si="1"/>
@@ -2639,20 +2653,21 @@
         <v>2B</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F45" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="4" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C46" s="2">
         <f t="shared" si="1"/>
@@ -2663,20 +2678,21 @@
         <v>2C</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F46" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="35"/>
+      <c r="H46" s="39"/>
+      <c r="I46" s="4" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C47" s="2">
         <f t="shared" si="1"/>
@@ -2687,20 +2703,21 @@
         <v>2D</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="35"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="4" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" si="1"/>
@@ -2711,20 +2728,21 @@
         <v>2E</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="35"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="4" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C49" s="2">
         <f t="shared" si="1"/>
@@ -2735,24 +2753,23 @@
         <v>2F</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F49" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="G49" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G49" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="I49" s="2"/>
-      <c r="J49" s="35"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="4" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C50" s="2">
         <f t="shared" si="1"/>
@@ -2763,24 +2780,23 @@
         <v>30</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F50" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="G50" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G50" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I50" s="2"/>
-      <c r="J50" s="35"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="4" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C51" s="2">
         <f t="shared" si="1"/>
@@ -2791,22 +2807,22 @@
         <v>31</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>213</v>
+        <v>306</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" s="2">
         <f t="shared" si="1"/>
@@ -2817,14 +2833,14 @@
         <v>32</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F52" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G52" s="20"/>
       <c r="H52" s="2" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2832,7 +2848,7 @@
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C53" s="2">
         <f t="shared" si="1"/>
@@ -2843,7 +2859,7 @@
         <v>33</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F53" s="20" t="s">
         <v>28</v>
@@ -2852,7 +2868,7 @@
         <v>33</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2860,7 +2876,7 @@
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C54" s="2">
         <f t="shared" si="1"/>
@@ -2871,12 +2887,12 @@
         <v>34</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -2884,7 +2900,7 @@
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" s="2">
         <f t="shared" si="1"/>
@@ -2895,12 +2911,12 @@
         <v>35</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -2908,30 +2924,30 @@
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="C56" s="2">
-        <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
       <c r="D56" s="17" t="str">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C57" s="13">
         <f t="shared" si="1"/>
@@ -2942,15 +2958,15 @@
         <v>37</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>112</v>
+        <v>311</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C58" s="13">
         <f t="shared" si="1"/>
@@ -2961,15 +2977,15 @@
         <v>38</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>111</v>
+        <v>157</v>
+      </c>
+      <c r="H58" s="20" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C59" s="15">
         <f t="shared" si="1"/>
@@ -2980,15 +2996,15 @@
         <v>39</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>234</v>
+        <v>307</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C60" s="15">
         <f t="shared" si="1"/>
@@ -2999,18 +3015,18 @@
         <v>3A</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>235</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C61" s="20">
         <f t="shared" si="1"/>
@@ -3021,7 +3037,7 @@
         <v>3B</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>17</v>
@@ -3030,13 +3046,13 @@
         <v>16</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C62" s="2">
         <f t="shared" ref="C62:C79" si="4">C61+1</f>
@@ -3047,7 +3063,7 @@
         <v>3C</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>17</v>
@@ -3056,13 +3072,13 @@
         <v>16</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C63" s="2">
         <f t="shared" si="4"/>
@@ -3073,7 +3089,7 @@
         <v>3D</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>17</v>
@@ -3082,13 +3098,13 @@
         <v>16</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C64" s="2">
         <f t="shared" si="4"/>
@@ -3099,7 +3115,7 @@
         <v>3E</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>17</v>
@@ -3108,13 +3124,13 @@
         <v>16</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="2" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C65" s="2">
         <f t="shared" si="4"/>
@@ -3125,7 +3141,7 @@
         <v>3F</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>17</v>
@@ -3134,13 +3150,13 @@
         <v>16</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="2" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C66" s="2">
         <f t="shared" si="4"/>
@@ -3151,7 +3167,7 @@
         <v>40</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>17</v>
@@ -3160,13 +3176,13 @@
         <v>16</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C67" s="2">
         <f t="shared" si="4"/>
@@ -3177,7 +3193,7 @@
         <v>41</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>17</v>
@@ -3186,13 +3202,13 @@
         <v>16</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="2" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C68" s="2">
         <f t="shared" si="4"/>
@@ -3203,7 +3219,7 @@
         <v>42</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>17</v>
@@ -3212,13 +3228,13 @@
         <v>16</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C69" s="2">
         <f t="shared" si="4"/>
@@ -3229,7 +3245,7 @@
         <v>43</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>17</v>
@@ -3238,13 +3254,13 @@
         <v>16</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C70" s="2">
         <f t="shared" si="4"/>
@@ -3255,7 +3271,7 @@
         <v>44</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>17</v>
@@ -3264,15 +3280,15 @@
         <v>16</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" t="s">
         <v>93</v>
-      </c>
-      <c r="B71" t="s">
-        <v>94</v>
       </c>
       <c r="C71" s="2">
         <f t="shared" si="4"/>
@@ -3283,7 +3299,7 @@
         <v>45</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>17</v>
@@ -3292,13 +3308,13 @@
         <v>16</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C72" s="2">
         <f t="shared" si="4"/>
@@ -3309,7 +3325,7 @@
         <v>46</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>17</v>
@@ -3318,13 +3334,13 @@
         <v>16</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C73" s="2">
         <f t="shared" si="4"/>
@@ -3335,7 +3351,7 @@
         <v>47</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>17</v>
@@ -3344,13 +3360,13 @@
         <v>16</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C74" s="2">
         <f t="shared" si="4"/>
@@ -3361,7 +3377,7 @@
         <v>48</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>17</v>
@@ -3370,15 +3386,15 @@
         <v>16</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="C75" s="20">
         <f t="shared" si="4"/>
@@ -3389,7 +3405,7 @@
         <v>49</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F75" s="20" t="s">
         <v>17</v>
@@ -3398,13 +3414,13 @@
         <v>16</v>
       </c>
       <c r="H75" s="20" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="20" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C76" s="20">
         <f t="shared" si="4"/>
@@ -3415,7 +3431,7 @@
         <v>4A</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F76" s="20" t="s">
         <v>17</v>
@@ -3424,13 +3440,13 @@
         <v>16</v>
       </c>
       <c r="H76" s="20" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="20" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="C77" s="20">
         <f t="shared" si="4"/>
@@ -3441,7 +3457,7 @@
         <v>4B</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F77" s="20" t="s">
         <v>17</v>
@@ -3450,13 +3466,13 @@
         <v>16</v>
       </c>
       <c r="H77" s="20" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="20" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="C78" s="20">
         <f t="shared" si="4"/>
@@ -3467,7 +3483,7 @@
         <v>4C</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F78" s="20" t="s">
         <v>17</v>
@@ -3476,15 +3492,15 @@
         <v>16</v>
       </c>
       <c r="H78" s="20" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="C79" s="20">
         <f t="shared" si="4"/>
@@ -3495,7 +3511,7 @@
         <v>4D</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F79"/>
       <c r="G79"/>
@@ -3603,8 +3619,12 @@
       <c r="H90" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="J42:J50"/>
+  <mergeCells count="5">
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="H42:H50"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="H33:H41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3635,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3643,13 +3663,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3658,13 +3678,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3673,13 +3693,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3688,13 +3708,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3703,13 +3723,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3718,13 +3738,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3733,13 +3753,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3748,18 +3768,18 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3767,13 +3787,13 @@
         <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3782,13 +3802,13 @@
         <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,13 +3817,13 @@
         <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
@@ -3819,8 +3839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3843,22 +3863,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3866,17 +3886,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="21" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G2" s="21"/>
       <c r="I2" s="24" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3885,7 +3905,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="21"/>
@@ -3893,7 +3913,7 @@
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="I3" s="25" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3902,7 +3922,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="21"/>
@@ -3910,7 +3930,7 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="I4" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3919,35 +3939,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="21"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3960,7 +3973,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3986,11 +3999,11 @@
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>86</v>
+      <c r="C2" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4001,8 +4014,8 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -4012,10 +4025,10 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" s="37"/>
+      <c r="C4" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="36"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -4025,8 +4038,8 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -4034,12 +4047,12 @@
         <v>4</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="D6" s="37"/>
+        <v>210</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
@@ -4047,10 +4060,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="37"/>
+        <v>211</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
@@ -4058,10 +4071,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D8" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4070,10 +4083,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4086,7 +4099,7 @@
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4095,10 +4108,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>238</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4107,13 +4120,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>140</v>
+        <v>97</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>133</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4122,9 +4135,9 @@
         <v>11</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="36"/>
+        <v>98</v>
+      </c>
+      <c r="C13" s="35"/>
       <c r="D13" s="32"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4133,11 +4146,11 @@
         <v>12</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4146,10 +4159,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4158,10 +4171,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4170,10 +4183,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4214,16 +4227,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4231,13 +4244,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4246,13 +4259,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>285</v>
+        <v>86</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4261,12 +4274,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>288</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>279</v>
-      </c>
-      <c r="D4" s="36"/>
+        <v>272</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
@@ -4274,10 +4287,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+        <v>229</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4286,12 +4299,12 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="36"/>
+        <v>230</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="35"/>
       <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4300,10 +4313,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+        <v>231</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4312,10 +4325,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>248</v>
-      </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
+        <v>232</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4324,10 +4337,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+        <v>233</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4336,10 +4349,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+        <v>234</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -4347,10 +4360,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+        <v>235</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
     </row>
     <row r="12" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
@@ -4358,10 +4371,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="36"/>
+        <v>273</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
@@ -4369,8 +4382,8 @@
         <v>12</v>
       </c>
       <c r="B13" s="20"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="35"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
@@ -4378,10 +4391,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="36"/>
+        <v>236</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="35"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
@@ -4389,12 +4402,12 @@
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>280</v>
-      </c>
-      <c r="D15" s="36"/>
+        <v>72</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
@@ -4402,10 +4415,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="36"/>
+        <v>101</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
@@ -4413,10 +4426,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="36"/>
+        <v>237</v>
+      </c>
+      <c r="C17" s="36"/>
+      <c r="D17" s="35"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -4424,12 +4437,12 @@
         <v>17</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>281</v>
-      </c>
-      <c r="D18" s="36"/>
+        <v>238</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="D18" s="35"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -4437,10 +4450,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>255</v>
-      </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
+        <v>239</v>
+      </c>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -4448,8 +4461,8 @@
         <v>19</v>
       </c>
       <c r="B20" s="20"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -4457,10 +4470,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
+        <v>240</v>
+      </c>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -4468,10 +4481,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
+        <v>241</v>
+      </c>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -4479,10 +4492,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
+        <v>242</v>
+      </c>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -4490,10 +4503,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
+        <v>243</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -4501,10 +4514,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
       <c r="E25" s="33"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -4513,10 +4526,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
+        <v>244</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
       <c r="E26" s="33"/>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4525,10 +4538,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="20"/>
-      <c r="C27" s="36" t="s">
-        <v>309</v>
-      </c>
-      <c r="D27" s="36"/>
+      <c r="C27" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="D27" s="35"/>
       <c r="E27" s="33"/>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4537,10 +4550,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
+        <v>245</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -4548,10 +4561,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
+        <v>274</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -4559,10 +4572,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
+        <v>275</v>
+      </c>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -4570,8 +4583,8 @@
         <v>30</v>
       </c>
       <c r="B31" s="20"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
@@ -4579,10 +4592,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+        <v>276</v>
+      </c>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
       <c r="E32" s="20"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -4591,10 +4604,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
+        <v>277</v>
+      </c>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -4602,10 +4615,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
+        <v>242</v>
+      </c>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
     </row>
     <row r="35" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
@@ -4613,10 +4626,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
+        <v>243</v>
+      </c>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
     </row>
     <row r="36" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
@@ -4624,10 +4637,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4636,17 +4649,17 @@
         <v>36</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
+        <v>278</v>
+      </c>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
     </row>
     <row r="38" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="D38" s="36"/>
+      <c r="D38" s="35"/>
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4655,12 +4668,12 @@
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="C39" s="36" t="s">
-        <v>310</v>
-      </c>
-      <c r="D39" s="36"/>
+        <v>279</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="D39" s="35"/>
     </row>
     <row r="40" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
@@ -4668,10 +4681,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
+        <v>280</v>
+      </c>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
     </row>
     <row r="41" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
@@ -4679,8 +4692,8 @@
         <v>40</v>
       </c>
       <c r="B41" s="20"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
     </row>
     <row r="42" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
@@ -4688,10 +4701,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
+        <v>281</v>
+      </c>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
     </row>
     <row r="43" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
@@ -4699,10 +4712,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>298</v>
-      </c>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
+        <v>282</v>
+      </c>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
       <c r="E43"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -4711,11 +4724,11 @@
         <v>43</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
+        <v>283</v>
+      </c>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
     </row>
     <row r="45" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
@@ -4723,11 +4736,11 @@
         <v>44</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
+        <v>284</v>
+      </c>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
     </row>
     <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
@@ -4735,11 +4748,11 @@
         <v>45</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
+        <v>285</v>
+      </c>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
@@ -4747,8 +4760,8 @@
         <v>46</v>
       </c>
       <c r="B47" s="20"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
@@ -4756,12 +4769,12 @@
         <v>47</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C48" s="36" t="s">
-        <v>282</v>
-      </c>
-      <c r="D48" s="36"/>
+        <v>72</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="D48" s="35"/>
       <c r="E48" s="14"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -4770,10 +4783,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
+        <v>102</v>
+      </c>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
@@ -4781,12 +4794,12 @@
         <v>49</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="C50" s="36" t="s">
-        <v>311</v>
-      </c>
-      <c r="D50" s="36"/>
+        <v>246</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="D50" s="35"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
@@ -4794,10 +4807,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
+        <v>242</v>
+      </c>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="20">
@@ -4805,10 +4818,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
+        <v>72</v>
+      </c>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
@@ -4816,10 +4829,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
+        <v>103</v>
+      </c>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
@@ -4827,7 +4840,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="20"/>
-      <c r="D54" s="36"/>
+      <c r="D54" s="35"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
@@ -4835,12 +4848,12 @@
         <v>54</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="C55" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="D55" s="36"/>
+        <v>286</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="35"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
@@ -4848,10 +4861,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
+        <v>287</v>
+      </c>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
@@ -4860,7 +4873,7 @@
       </c>
       <c r="B57" s="20"/>
       <c r="C57" s="33"/>
-      <c r="D57" s="36"/>
+      <c r="D57" s="35"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
@@ -4868,12 +4881,12 @@
         <v>57</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>263</v>
-      </c>
-      <c r="C58" s="36" t="s">
-        <v>283</v>
-      </c>
-      <c r="D58" s="36"/>
+        <v>247</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="D58" s="35"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
@@ -4881,10 +4894,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
+        <v>229</v>
+      </c>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="20">
@@ -4892,8 +4905,8 @@
         <v>59</v>
       </c>
       <c r="B60" s="20"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
@@ -4901,13 +4914,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
+        <v>108</v>
+      </c>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="20">
@@ -4915,13 +4928,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
+        <v>153</v>
+      </c>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
@@ -4929,13 +4942,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="C63" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
+        <v>248</v>
+      </c>
+      <c r="C63" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="20">
@@ -4943,11 +4956,11 @@
         <v>63</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
+        <v>249</v>
+      </c>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="20">
@@ -4955,8 +4968,8 @@
         <v>64</v>
       </c>
       <c r="B65" s="20"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="20">
@@ -4964,13 +4977,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>266</v>
-      </c>
-      <c r="C66" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
+        <v>250</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66" s="35"/>
+      <c r="E66" s="35"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="20">
@@ -4978,11 +4991,11 @@
         <v>66</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
+        <v>251</v>
+      </c>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="20">
@@ -4990,11 +5003,11 @@
         <v>67</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
+        <v>252</v>
+      </c>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="20">
@@ -5002,10 +5015,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
+        <v>253</v>
+      </c>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="20">
@@ -5013,10 +5026,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
+        <v>254</v>
+      </c>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="20">
@@ -5024,7 +5037,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="20"/>
-      <c r="D71" s="36"/>
+      <c r="D71" s="35"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="20">
@@ -5032,13 +5045,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C72" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="D72" s="39" t="s">
-        <v>118</v>
+        <v>107</v>
+      </c>
+      <c r="C72" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D72" s="38" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -5047,10 +5060,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="C73" s="36"/>
-      <c r="D73" s="39"/>
+        <v>255</v>
+      </c>
+      <c r="C73" s="35"/>
+      <c r="D73" s="38"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="20">
@@ -5058,12 +5071,12 @@
         <v>73</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="C74" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="D74" s="39"/>
+        <v>110</v>
+      </c>
+      <c r="D74" s="38"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="20">
@@ -5071,12 +5084,12 @@
         <v>74</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>248</v>
-      </c>
-      <c r="C75" s="36" t="s">
-        <v>312</v>
-      </c>
-      <c r="D75" s="39"/>
+        <v>232</v>
+      </c>
+      <c r="C75" s="35" t="s">
+        <v>296</v>
+      </c>
+      <c r="D75" s="38"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
@@ -5084,10 +5097,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="C76" s="36"/>
-      <c r="D76" s="39"/>
+        <v>233</v>
+      </c>
+      <c r="C76" s="35"/>
+      <c r="D76" s="38"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
@@ -5095,12 +5108,12 @@
         <v>76</v>
       </c>
       <c r="B77" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="C77" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="D77" s="39"/>
+        <v>257</v>
+      </c>
+      <c r="C77" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D77" s="38"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
@@ -5108,10 +5121,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>274</v>
-      </c>
-      <c r="C78" s="36"/>
-      <c r="D78" s="39"/>
+        <v>258</v>
+      </c>
+      <c r="C78" s="35"/>
+      <c r="D78" s="38"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
@@ -5119,10 +5132,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="20" t="s">
-        <v>306</v>
-      </c>
-      <c r="C79" s="36"/>
-      <c r="D79" s="39"/>
+        <v>290</v>
+      </c>
+      <c r="C79" s="35"/>
+      <c r="D79" s="38"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
@@ -5130,12 +5143,12 @@
         <v>79</v>
       </c>
       <c r="B80" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="C80" s="36" t="s">
-        <v>313</v>
-      </c>
-      <c r="D80" s="39"/>
+        <v>259</v>
+      </c>
+      <c r="C80" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="D80" s="38"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="20">
@@ -5143,10 +5156,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="C81" s="36"/>
-      <c r="D81" s="39"/>
+        <v>291</v>
+      </c>
+      <c r="C81" s="35"/>
+      <c r="D81" s="38"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="20">
@@ -5154,10 +5167,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="20" t="s">
-        <v>308</v>
-      </c>
-      <c r="C82" s="36"/>
-      <c r="D82" s="39"/>
+        <v>292</v>
+      </c>
+      <c r="C82" s="35"/>
+      <c r="D82" s="38"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="20">
@@ -5165,10 +5178,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="C83" s="36"/>
-      <c r="D83" s="39"/>
+        <v>260</v>
+      </c>
+      <c r="C83" s="35"/>
+      <c r="D83" s="38"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="20">
@@ -5176,10 +5189,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C84" s="36"/>
-      <c r="D84" s="39"/>
+        <v>106</v>
+      </c>
+      <c r="C84" s="35"/>
+      <c r="D84" s="38"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
@@ -5187,10 +5200,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="C85" s="36"/>
-      <c r="D85" s="39"/>
+        <v>261</v>
+      </c>
+      <c r="C85" s="35"/>
+      <c r="D85" s="38"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="20">
@@ -5198,20 +5211,30 @@
         <v>85</v>
       </c>
       <c r="B86" s="20" t="s">
-        <v>306</v>
-      </c>
-      <c r="C86" s="36"/>
+        <v>290</v>
+      </c>
+      <c r="C86" s="35"/>
       <c r="D86" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C87" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="D72:D85"/>
+    <mergeCell ref="D3:D71"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="E60:E68"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C58:C59"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E44:E47"/>
     <mergeCell ref="C66:C70"/>
@@ -5221,18 +5244,8 @@
     <mergeCell ref="C18:C26"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="E60:E68"/>
     <mergeCell ref="C27:C37"/>
     <mergeCell ref="C39:C46"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="D72:D85"/>
-    <mergeCell ref="D3:D71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5243,7 +5256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -5258,89 +5271,89 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
store bootloader offset at end of bootloader
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doridian\Documents\Visual Studio 2017\Projects\HMCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{42A4A329-2AAF-420D-9EAF-B75F66DEC3FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CDC5D5C2-3012-42BA-85AD-D1FEA96B3481}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -926,12 +926,6 @@
     <t>Turn on ROM encryption and return and jump</t>
   </si>
   <si>
-    <t>END</t>
-  </si>
-  <si>
-    <t>SIZE / 2</t>
-  </si>
-  <si>
     <t>BOOTLOADEREND</t>
   </si>
   <si>
@@ -999,6 +993,12 @@
   </si>
   <si>
     <t>Check if FLAG_LT</t>
+  </si>
+  <si>
+    <t>RAMEND</t>
+  </si>
+  <si>
+    <t>RAMEND - BL_OFFSET</t>
   </si>
 </sst>
 </file>
@@ -1503,7 +1503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
@@ -1668,7 +1668,7 @@
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
         <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1713,7 +1713,7 @@
         <v>28</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1736,7 +1736,7 @@
         <v>28</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2198,7 +2198,7 @@
         <v>143</v>
       </c>
       <c r="I27" s="35" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2378,7 +2378,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="35"/>
       <c r="I34" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J34" s="2"/>
     </row>
@@ -2404,7 +2404,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="35"/>
       <c r="I35" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J35" s="2"/>
     </row>
@@ -2430,7 +2430,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="35"/>
       <c r="I36" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J36" s="2"/>
     </row>
@@ -2456,7 +2456,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="35"/>
       <c r="I37" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J37" s="2"/>
     </row>
@@ -2480,7 +2480,7 @@
       </c>
       <c r="H38" s="35"/>
       <c r="I38" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2505,7 +2505,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="35"/>
       <c r="I39" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J39" s="2"/>
     </row>
@@ -2526,14 +2526,14 @@
         <v>156</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>28</v>
       </c>
       <c r="H40" s="35"/>
       <c r="I40" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J40" s="2"/>
     </row>
@@ -2554,14 +2554,14 @@
         <v>156</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>28</v>
       </c>
       <c r="H41" s="35"/>
       <c r="I41" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J41" s="2"/>
     </row>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="G42" s="20"/>
       <c r="H42" s="39" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2611,7 +2611,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="39"/>
       <c r="I43" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2636,7 +2636,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="39"/>
       <c r="I44" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2661,7 +2661,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="39"/>
       <c r="I45" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2686,7 +2686,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="39"/>
       <c r="I46" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2711,7 +2711,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="39"/>
       <c r="I47" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2736,7 +2736,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="39"/>
       <c r="I48" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2756,14 +2756,14 @@
         <v>156</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="H49" s="39"/>
       <c r="I49" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2783,14 +2783,14 @@
         <v>156</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>28</v>
       </c>
       <c r="H50" s="39"/>
       <c r="I50" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2812,7 +2812,7 @@
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2961,7 +2961,7 @@
         <v>157</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
         <v>157</v>
       </c>
       <c r="H58" s="20" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2999,7 +2999,7 @@
         <v>157</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3018,7 +3018,7 @@
         <v>157</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -3839,7 +3839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -4111,7 +4111,7 @@
         <v>222</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5256,8 +5256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5298,8 +5298,8 @@
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>299</v>
+      <c r="A5" s="9" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5307,13 +5307,13 @@
         <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5353,7 +5353,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>298</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add POPNIL, POPNIL64, RETNA
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doridian\Documents\Visual Studio 2017\Projects\HMCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2798F87D-6235-4AE8-BDBB-9A7B4773A53E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D6FABA59-91AA-464C-96DA-875AB2553601}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="329">
   <si>
     <t>Name</t>
   </si>
@@ -999,6 +999,24 @@
   </si>
   <si>
     <t>ENC Bootloader at RAM_SIZE - 4096</t>
+  </si>
+  <si>
+    <t>RETNA</t>
+  </si>
+  <si>
+    <t>POPNIL</t>
+  </si>
+  <si>
+    <t>POPNIL64</t>
+  </si>
+  <si>
+    <t>CSP += 4</t>
+  </si>
+  <si>
+    <t>CSP += 8</t>
+  </si>
+  <si>
+    <t>RETN, CSP += 4 * Reg</t>
   </si>
 </sst>
 </file>
@@ -1172,17 +1190,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1503,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="17" t="str">
-        <f t="shared" ref="D3:D60" si="0">DEC2HEX(C3,2)</f>
+        <f t="shared" ref="D3:D51" si="0">DEC2HEX(C3,2)</f>
         <v>01</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -1676,7 +1694,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" ref="C7:C61" si="1">C6+1</f>
+        <f t="shared" ref="C7:C51" si="1">C6+1</f>
         <v>5</v>
       </c>
       <c r="D7" s="17" t="str">
@@ -2585,7 +2603,7 @@
         <v>28</v>
       </c>
       <c r="G42" s="20"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="36" t="s">
         <v>305</v>
       </c>
     </row>
@@ -2609,7 +2627,7 @@
         <v>28</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="H43" s="39"/>
+      <c r="H43" s="36"/>
       <c r="I43" s="4" t="s">
         <v>310</v>
       </c>
@@ -2634,7 +2652,7 @@
         <v>28</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="H44" s="39"/>
+      <c r="H44" s="36"/>
       <c r="I44" s="4" t="s">
         <v>311</v>
       </c>
@@ -2659,7 +2677,7 @@
         <v>28</v>
       </c>
       <c r="G45" s="2"/>
-      <c r="H45" s="39"/>
+      <c r="H45" s="36"/>
       <c r="I45" s="4" t="s">
         <v>315</v>
       </c>
@@ -2684,7 +2702,7 @@
         <v>28</v>
       </c>
       <c r="G46" s="2"/>
-      <c r="H46" s="39"/>
+      <c r="H46" s="36"/>
       <c r="I46" s="4" t="s">
         <v>316</v>
       </c>
@@ -2709,7 +2727,7 @@
         <v>28</v>
       </c>
       <c r="G47" s="2"/>
-      <c r="H47" s="39"/>
+      <c r="H47" s="36"/>
       <c r="I47" s="4" t="s">
         <v>317</v>
       </c>
@@ -2734,7 +2752,7 @@
         <v>28</v>
       </c>
       <c r="G48" s="2"/>
-      <c r="H48" s="39"/>
+      <c r="H48" s="36"/>
       <c r="I48" s="4" t="s">
         <v>318</v>
       </c>
@@ -2761,7 +2779,7 @@
       <c r="G49" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H49" s="39"/>
+      <c r="H49" s="36"/>
       <c r="I49" s="4" t="s">
         <v>313</v>
       </c>
@@ -2788,7 +2806,7 @@
       <c r="G50" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H50" s="39"/>
+      <c r="H50" s="36"/>
       <c r="I50" s="4" t="s">
         <v>314</v>
       </c>
@@ -2825,11 +2843,11 @@
         <v>47</v>
       </c>
       <c r="C52" s="2">
-        <f t="shared" si="1"/>
+        <f>C51+1</f>
         <v>50</v>
       </c>
       <c r="D52" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C52,2)</f>
         <v>32</v>
       </c>
       <c r="E52" s="9" t="s">
@@ -2851,11 +2869,11 @@
         <v>49</v>
       </c>
       <c r="C53" s="2">
-        <f t="shared" si="1"/>
+        <f>C52+1</f>
         <v>51</v>
       </c>
       <c r="D53" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C53,2)</f>
         <v>33</v>
       </c>
       <c r="E53" s="9" t="s">
@@ -2879,11 +2897,11 @@
         <v>48</v>
       </c>
       <c r="C54" s="2">
-        <f t="shared" si="1"/>
+        <f>C53+1</f>
         <v>52</v>
       </c>
       <c r="D54" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C54,2)</f>
         <v>34</v>
       </c>
       <c r="E54" s="9" t="s">
@@ -2903,11 +2921,11 @@
         <v>50</v>
       </c>
       <c r="C55" s="2">
-        <f t="shared" si="1"/>
+        <f>C54+1</f>
         <v>53</v>
       </c>
       <c r="D55" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C55,2)</f>
         <v>35</v>
       </c>
       <c r="E55" s="9" t="s">
@@ -2927,11 +2945,11 @@
         <v>53</v>
       </c>
       <c r="C56" s="2">
-        <f t="shared" si="1"/>
+        <f>C55+1</f>
         <v>54</v>
       </c>
       <c r="D56" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C56,2)</f>
         <v>36</v>
       </c>
       <c r="E56" s="9" t="s">
@@ -2950,11 +2968,11 @@
         <v>107</v>
       </c>
       <c r="C57" s="13">
-        <f t="shared" si="1"/>
+        <f>C56+1</f>
         <v>55</v>
       </c>
       <c r="D57" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C57,2)</f>
         <v>37</v>
       </c>
       <c r="E57" s="9" t="s">
@@ -2969,11 +2987,11 @@
         <v>106</v>
       </c>
       <c r="C58" s="13">
-        <f t="shared" si="1"/>
+        <f>C57+1</f>
         <v>56</v>
       </c>
       <c r="D58" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C58,2)</f>
         <v>38</v>
       </c>
       <c r="E58" s="9" t="s">
@@ -2988,11 +3006,11 @@
         <v>115</v>
       </c>
       <c r="C59" s="15">
-        <f t="shared" si="1"/>
+        <f>C58+1</f>
         <v>57</v>
       </c>
       <c r="D59" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C59,2)</f>
         <v>39</v>
       </c>
       <c r="E59" s="9" t="s">
@@ -3007,11 +3025,11 @@
         <v>116</v>
       </c>
       <c r="C60" s="15">
-        <f t="shared" si="1"/>
+        <f>C59+1</f>
         <v>58</v>
       </c>
       <c r="D60" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(C60,2)</f>
         <v>3A</v>
       </c>
       <c r="E60" s="9" t="s">
@@ -3029,7 +3047,7 @@
         <v>184</v>
       </c>
       <c r="C61" s="20">
-        <f t="shared" si="1"/>
+        <f>C60+1</f>
         <v>59</v>
       </c>
       <c r="D61" s="17" t="str">
@@ -3055,7 +3073,7 @@
         <v>185</v>
       </c>
       <c r="C62" s="2">
-        <f t="shared" ref="C62:C79" si="4">C61+1</f>
+        <f t="shared" ref="C62:C82" si="4">C61+1</f>
         <v>60</v>
       </c>
       <c r="D62" s="17" t="str">
@@ -3453,7 +3471,7 @@
         <v>75</v>
       </c>
       <c r="D77" s="17" t="str">
-        <f t="shared" ref="D77:D79" si="6">DEC2HEX(C77,2)</f>
+        <f t="shared" ref="D77:D81" si="6">DEC2HEX(C77,2)</f>
         <v>4B</v>
       </c>
       <c r="E77" s="9" t="s">
@@ -3519,25 +3537,69 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="20"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="20"/>
+      <c r="B80" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C80" s="20">
+        <f t="shared" si="4"/>
+        <v>78</v>
+      </c>
+      <c r="D80" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v>4E</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="G80" s="20"/>
-      <c r="H80" s="20"/>
+      <c r="H80" s="20" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="20"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="9"/>
+      <c r="B81" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="C81" s="20">
+        <f t="shared" si="4"/>
+        <v>79</v>
+      </c>
+      <c r="D81" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v>4F</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>157</v>
+      </c>
       <c r="F81" s="20"/>
       <c r="G81" s="20"/>
-      <c r="H81" s="20"/>
-    </row>
-    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H81" s="20" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="C82" s="20">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="D82" s="17" t="str">
+        <f t="shared" ref="D82" si="7">DEC2HEX(C82,2)</f>
+        <v>50</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="H82" t="s">
+        <v>327</v>
+      </c>
+    </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="20"/>
       <c r="B83" s="20"/>
@@ -3901,7 +3963,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
-        <f t="shared" ref="A3:A6" si="0">A2+1</f>
+        <f t="shared" ref="A3:A5" si="0">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -4002,7 +4064,7 @@
       <c r="C2" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4015,7 +4077,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
+      <c r="D3" s="37"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -4028,7 +4090,7 @@
       <c r="C4" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="37"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -4039,7 +4101,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="35"/>
-      <c r="D5" s="36"/>
+      <c r="D5" s="37"/>
     </row>
     <row r="6" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -4052,7 +4114,7 @@
       <c r="C6" s="35" t="s">
         <v>212</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="37"/>
     </row>
     <row r="7" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
@@ -4063,7 +4125,7 @@
         <v>211</v>
       </c>
       <c r="C7" s="35"/>
-      <c r="D7" s="36"/>
+      <c r="D7" s="37"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
@@ -4212,7 +4274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -4373,7 +4435,7 @@
       <c r="B12" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4382,7 +4444,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="20"/>
-      <c r="C13" s="37"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="35"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -4393,7 +4455,7 @@
       <c r="B14" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="C14" s="37"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="35"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -4404,7 +4466,7 @@
       <c r="B15" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="37" t="s">
         <v>262</v>
       </c>
       <c r="D15" s="35"/>
@@ -4417,7 +4479,7 @@
       <c r="B16" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -4428,7 +4490,7 @@
       <c r="B17" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="C17" s="36"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="35"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -5225,13 +5287,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="D72:D85"/>
-    <mergeCell ref="D3:D71"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C75:C76"/>
     <mergeCell ref="E60:E68"/>
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="C58:C59"/>
@@ -5246,6 +5301,13 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C27:C37"/>
     <mergeCell ref="C39:C46"/>
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="D72:D85"/>
+    <mergeCell ref="D3:D71"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C75:C76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add U8U8, U8, I8, I8I8
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doridian\Documents\Visual Studio 2017\Projects\HMCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9F411E1E-AE0B-44D8-B630-589661217872}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9CD801EE-D129-486E-A162-BC398492B78D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1004,9 +1004,6 @@
     <t>RETNA</t>
   </si>
   <si>
-    <t>V8</t>
-  </si>
-  <si>
     <t>POPNIL</t>
   </si>
   <si>
@@ -1029,6 +1026,9 @@
   </si>
   <si>
     <t>RETN, CSP += Reg</t>
+  </si>
+  <si>
+    <t>U8</t>
   </si>
 </sst>
 </file>
@@ -1209,10 +1209,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1534,7 +1534,7 @@
   <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,11 +2855,11 @@
         <v>47</v>
       </c>
       <c r="C52" s="2">
-        <f>C51+1</f>
+        <f t="shared" ref="C52:C61" si="3">C51+1</f>
         <v>50</v>
       </c>
       <c r="D52" s="17" t="str">
-        <f>DEC2HEX(C52,2)</f>
+        <f t="shared" ref="D52:D60" si="4">DEC2HEX(C52,2)</f>
         <v>32</v>
       </c>
       <c r="E52" s="9" t="s">
@@ -2881,11 +2881,11 @@
         <v>49</v>
       </c>
       <c r="C53" s="2">
-        <f>C52+1</f>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="D53" s="17" t="str">
-        <f>DEC2HEX(C53,2)</f>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="E53" s="9" t="s">
@@ -2909,11 +2909,11 @@
         <v>48</v>
       </c>
       <c r="C54" s="2">
-        <f>C53+1</f>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="D54" s="17" t="str">
-        <f>DEC2HEX(C54,2)</f>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="E54" s="9" t="s">
@@ -2933,11 +2933,11 @@
         <v>50</v>
       </c>
       <c r="C55" s="2">
-        <f>C54+1</f>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="D55" s="17" t="str">
-        <f>DEC2HEX(C55,2)</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="E55" s="9" t="s">
@@ -2957,11 +2957,11 @@
         <v>53</v>
       </c>
       <c r="C56" s="2">
-        <f>C55+1</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="D56" s="17" t="str">
-        <f>DEC2HEX(C56,2)</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="E56" s="9" t="s">
@@ -2980,11 +2980,11 @@
         <v>107</v>
       </c>
       <c r="C57" s="13">
-        <f>C56+1</f>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="D57" s="17" t="str">
-        <f>DEC2HEX(C57,2)</f>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="E57" s="9" t="s">
@@ -2999,11 +2999,11 @@
         <v>106</v>
       </c>
       <c r="C58" s="13">
-        <f>C57+1</f>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="D58" s="17" t="str">
-        <f>DEC2HEX(C58,2)</f>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="E58" s="9" t="s">
@@ -3018,11 +3018,11 @@
         <v>115</v>
       </c>
       <c r="C59" s="15">
-        <f>C58+1</f>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="D59" s="17" t="str">
-        <f>DEC2HEX(C59,2)</f>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="E59" s="9" t="s">
@@ -3037,11 +3037,11 @@
         <v>116</v>
       </c>
       <c r="C60" s="15">
-        <f>C59+1</f>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="D60" s="17" t="str">
-        <f>DEC2HEX(C60,2)</f>
+        <f t="shared" si="4"/>
         <v>3A</v>
       </c>
       <c r="E60" s="9" t="s">
@@ -3059,11 +3059,11 @@
         <v>184</v>
       </c>
       <c r="C61" s="20">
-        <f>C60+1</f>
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="D61" s="17" t="str">
-        <f t="shared" ref="D61:D72" si="3">DEC2HEX(C61,2)</f>
+        <f t="shared" ref="D61:D72" si="5">DEC2HEX(C61,2)</f>
         <v>3B</v>
       </c>
       <c r="E61" s="9" t="s">
@@ -3085,11 +3085,11 @@
         <v>185</v>
       </c>
       <c r="C62" s="2">
-        <f t="shared" ref="C62:C83" si="4">C61+1</f>
+        <f t="shared" ref="C62:C83" si="6">C61+1</f>
         <v>60</v>
       </c>
       <c r="D62" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3C</v>
       </c>
       <c r="E62" s="9" t="s">
@@ -3111,11 +3111,11 @@
         <v>186</v>
       </c>
       <c r="C63" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="D63" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3D</v>
       </c>
       <c r="E63" s="9" t="s">
@@ -3137,11 +3137,11 @@
         <v>187</v>
       </c>
       <c r="C64" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>62</v>
       </c>
       <c r="D64" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3E</v>
       </c>
       <c r="E64" s="9" t="s">
@@ -3163,11 +3163,11 @@
         <v>188</v>
       </c>
       <c r="C65" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>63</v>
       </c>
       <c r="D65" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3F</v>
       </c>
       <c r="E65" s="9" t="s">
@@ -3189,11 +3189,11 @@
         <v>189</v>
       </c>
       <c r="C66" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="D66" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="E66" s="9" t="s">
@@ -3215,11 +3215,11 @@
         <v>190</v>
       </c>
       <c r="C67" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
       <c r="D67" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="E67" s="9" t="s">
@@ -3241,11 +3241,11 @@
         <v>191</v>
       </c>
       <c r="C68" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
       <c r="D68" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="E68" s="9" t="s">
@@ -3267,11 +3267,11 @@
         <v>192</v>
       </c>
       <c r="C69" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>67</v>
       </c>
       <c r="D69" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="E69" s="9" t="s">
@@ -3293,11 +3293,11 @@
         <v>193</v>
       </c>
       <c r="C70" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
       <c r="D70" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="E70" s="9" t="s">
@@ -3321,11 +3321,11 @@
         <v>93</v>
       </c>
       <c r="C71" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
       <c r="D71" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="E71" s="9" t="s">
@@ -3347,11 +3347,11 @@
         <v>94</v>
       </c>
       <c r="C72" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="D72" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
       <c r="E72" s="9" t="s">
@@ -3373,11 +3373,11 @@
         <v>95</v>
       </c>
       <c r="C73" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>71</v>
       </c>
       <c r="D73" s="17" t="str">
-        <f t="shared" ref="D73:D76" si="5">DEC2HEX(C73,2)</f>
+        <f t="shared" ref="D73:D76" si="7">DEC2HEX(C73,2)</f>
         <v>47</v>
       </c>
       <c r="E73" s="9" t="s">
@@ -3399,11 +3399,11 @@
         <v>96</v>
       </c>
       <c r="C74" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>72</v>
       </c>
       <c r="D74" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="E74" s="9" t="s">
@@ -3427,11 +3427,11 @@
         <v>217</v>
       </c>
       <c r="C75" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>73</v>
       </c>
       <c r="D75" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="E75" s="9" t="s">
@@ -3453,11 +3453,11 @@
         <v>218</v>
       </c>
       <c r="C76" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>74</v>
       </c>
       <c r="D76" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4A</v>
       </c>
       <c r="E76" s="9" t="s">
@@ -3479,11 +3479,11 @@
         <v>220</v>
       </c>
       <c r="C77" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="D77" s="17" t="str">
-        <f t="shared" ref="D77:D81" si="6">DEC2HEX(C77,2)</f>
+        <f t="shared" ref="D77:D81" si="8">DEC2HEX(C77,2)</f>
         <v>4B</v>
       </c>
       <c r="E77" s="9" t="s">
@@ -3505,11 +3505,11 @@
         <v>219</v>
       </c>
       <c r="C78" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="D78" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4C</v>
       </c>
       <c r="E78" s="9" t="s">
@@ -3533,11 +3533,11 @@
         <v>209</v>
       </c>
       <c r="C79" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>77</v>
       </c>
       <c r="D79" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4D</v>
       </c>
       <c r="E79" s="9" t="s">
@@ -3553,11 +3553,11 @@
         <v>323</v>
       </c>
       <c r="C80" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>78</v>
       </c>
       <c r="D80" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4E</v>
       </c>
       <c r="E80" s="9" t="s">
@@ -3568,20 +3568,20 @@
       </c>
       <c r="G80" s="20"/>
       <c r="H80" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="20"/>
       <c r="B81" s="20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C81" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>79</v>
       </c>
       <c r="D81" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4F</v>
       </c>
       <c r="E81" s="9" t="s">
@@ -3590,50 +3590,50 @@
       <c r="F81" s="20"/>
       <c r="G81" s="20"/>
       <c r="H81" s="20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C82" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="D82" s="17" t="str">
-        <f t="shared" ref="D82:D83" si="7">DEC2HEX(C82,2)</f>
+        <f t="shared" ref="D82:D83" si="9">DEC2HEX(C82,2)</f>
         <v>50</v>
       </c>
       <c r="E82" s="9" t="s">
         <v>157</v>
       </c>
       <c r="H82" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="20"/>
       <c r="B83" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="C83" s="20">
+        <f t="shared" si="6"/>
+        <v>81</v>
+      </c>
+      <c r="D83" s="17" t="str">
+        <f t="shared" si="9"/>
+        <v>51</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="F83" s="20" t="s">
         <v>329</v>
-      </c>
-      <c r="C83" s="20">
-        <f t="shared" si="4"/>
-        <v>81</v>
-      </c>
-      <c r="D83" s="17" t="str">
-        <f t="shared" si="7"/>
-        <v>51</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="F83" s="20" t="s">
-        <v>330</v>
       </c>
       <c r="G83" s="20"/>
       <c r="H83" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
       <c r="B12" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="C12" s="39"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4470,7 +4470,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="20"/>
-      <c r="C13" s="39"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="35"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -4481,7 +4481,7 @@
       <c r="B14" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="35"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -5138,7 +5138,7 @@
       <c r="C72" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="D72" s="38" t="s">
+      <c r="D72" s="39" t="s">
         <v>113</v>
       </c>
     </row>
@@ -5151,7 +5151,7 @@
         <v>254</v>
       </c>
       <c r="C73" s="35"/>
-      <c r="D73" s="38"/>
+      <c r="D73" s="39"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="20">
@@ -5164,7 +5164,7 @@
       <c r="C74" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="D74" s="38"/>
+      <c r="D74" s="39"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="20">
@@ -5177,7 +5177,7 @@
       <c r="C75" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="D75" s="38"/>
+      <c r="D75" s="39"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
@@ -5188,7 +5188,7 @@
         <v>232</v>
       </c>
       <c r="C76" s="35"/>
-      <c r="D76" s="38"/>
+      <c r="D76" s="39"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
@@ -5201,7 +5201,7 @@
       <c r="C77" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="D77" s="38"/>
+      <c r="D77" s="39"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
@@ -5212,7 +5212,7 @@
         <v>257</v>
       </c>
       <c r="C78" s="35"/>
-      <c r="D78" s="38"/>
+      <c r="D78" s="39"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
@@ -5223,7 +5223,7 @@
         <v>288</v>
       </c>
       <c r="C79" s="35"/>
-      <c r="D79" s="38"/>
+      <c r="D79" s="39"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
@@ -5236,7 +5236,7 @@
       <c r="C80" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="D80" s="38"/>
+      <c r="D80" s="39"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="20">
@@ -5247,7 +5247,7 @@
         <v>289</v>
       </c>
       <c r="C81" s="35"/>
-      <c r="D81" s="38"/>
+      <c r="D81" s="39"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="20">
@@ -5258,7 +5258,7 @@
         <v>290</v>
       </c>
       <c r="C82" s="35"/>
-      <c r="D82" s="38"/>
+      <c r="D82" s="39"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="20">
@@ -5269,7 +5269,7 @@
         <v>259</v>
       </c>
       <c r="C83" s="35"/>
-      <c r="D83" s="38"/>
+      <c r="D83" s="39"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="20">
@@ -5280,7 +5280,7 @@
         <v>106</v>
       </c>
       <c r="C84" s="35"/>
-      <c r="D84" s="38"/>
+      <c r="D84" s="39"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
@@ -5291,7 +5291,7 @@
         <v>260</v>
       </c>
       <c r="C85" s="35"/>
-      <c r="D85" s="38"/>
+      <c r="D85" s="39"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="20">
@@ -5313,6 +5313,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="D72:D85"/>
+    <mergeCell ref="D3:D71"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C75:C76"/>
     <mergeCell ref="E60:E68"/>
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="C58:C59"/>
@@ -5327,13 +5334,6 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C27:C37"/>
     <mergeCell ref="C39:C46"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="D72:D85"/>
-    <mergeCell ref="D3:D71"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C75:C76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
allow for dynamic RAM size, relocatable bootloader
</commit_message>
<xml_diff>
--- a/docs/CPU.xlsx
+++ b/docs/CPU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doridian\Documents\Visual Studio 2017\Projects\HMCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B2BBA2AD-A9BA-42F5-A43B-5D5A6242BFD9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{91C4AEF9-A79E-464F-BB7E-1444173144D7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="339">
   <si>
     <t>Name</t>
   </si>
@@ -1035,6 +1035,18 @@
   </si>
   <si>
     <t>RegDst[0:15] = RegSrc &amp; 0xFFFF</t>
+  </si>
+  <si>
+    <t>CPUID</t>
+  </si>
+  <si>
+    <t>Reg = CPUID</t>
+  </si>
+  <si>
+    <t>RAMSIZE</t>
+  </si>
+  <si>
+    <t>Reg= RAMSIZE</t>
   </si>
 </sst>
 </file>
@@ -1215,10 +1227,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1539,8 +1551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3091,7 +3103,7 @@
         <v>185</v>
       </c>
       <c r="C62" s="2">
-        <f t="shared" ref="C62:C83" si="6">C61+1</f>
+        <f t="shared" ref="C62:C85" si="6">C61+1</f>
         <v>60</v>
       </c>
       <c r="D62" s="17" t="str">
@@ -3608,7 +3620,7 @@
         <v>80</v>
       </c>
       <c r="D82" s="17" t="str">
-        <f t="shared" ref="D82:D83" si="9">DEC2HEX(C82,2)</f>
+        <f t="shared" ref="D82:D85" si="9">DEC2HEX(C82,2)</f>
         <v>50</v>
       </c>
       <c r="E82" s="9" t="s">
@@ -3644,23 +3656,51 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="20"/>
+      <c r="B84" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="C84" s="20">
+        <f t="shared" si="6"/>
+        <v>82</v>
+      </c>
+      <c r="D84" s="17" t="str">
+        <f t="shared" si="9"/>
+        <v>52</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="G84" s="20"/>
-      <c r="H84" s="20"/>
+      <c r="H84" s="20" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="20"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="20"/>
+      <c r="B85" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="C85" s="20">
+        <f t="shared" si="6"/>
+        <v>83</v>
+      </c>
+      <c r="D85" s="17" t="str">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F85" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="G85" s="20"/>
-      <c r="H85" s="20"/>
+      <c r="H85" s="20" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="20"/>
@@ -4467,7 +4507,7 @@
       <c r="B12" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="C12" s="39"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4476,7 +4516,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="20"/>
-      <c r="C13" s="39"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="35"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -4487,7 +4527,7 @@
       <c r="B14" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="35"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -5144,7 +5184,7 @@
       <c r="C72" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="D72" s="38" t="s">
+      <c r="D72" s="39" t="s">
         <v>113</v>
       </c>
     </row>
@@ -5157,7 +5197,7 @@
         <v>254</v>
       </c>
       <c r="C73" s="35"/>
-      <c r="D73" s="38"/>
+      <c r="D73" s="39"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="20">
@@ -5170,7 +5210,7 @@
       <c r="C74" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="D74" s="38"/>
+      <c r="D74" s="39"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="20">
@@ -5183,7 +5223,7 @@
       <c r="C75" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="D75" s="38"/>
+      <c r="D75" s="39"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
@@ -5194,7 +5234,7 @@
         <v>232</v>
       </c>
       <c r="C76" s="35"/>
-      <c r="D76" s="38"/>
+      <c r="D76" s="39"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
@@ -5207,7 +5247,7 @@
       <c r="C77" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="D77" s="38"/>
+      <c r="D77" s="39"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
@@ -5218,7 +5258,7 @@
         <v>257</v>
       </c>
       <c r="C78" s="35"/>
-      <c r="D78" s="38"/>
+      <c r="D78" s="39"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
@@ -5229,7 +5269,7 @@
         <v>288</v>
       </c>
       <c r="C79" s="35"/>
-      <c r="D79" s="38"/>
+      <c r="D79" s="39"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
@@ -5242,7 +5282,7 @@
       <c r="C80" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="D80" s="38"/>
+      <c r="D80" s="39"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="20">
@@ -5253,7 +5293,7 @@
         <v>289</v>
       </c>
       <c r="C81" s="35"/>
-      <c r="D81" s="38"/>
+      <c r="D81" s="39"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="20">
@@ -5264,7 +5304,7 @@
         <v>290</v>
       </c>
       <c r="C82" s="35"/>
-      <c r="D82" s="38"/>
+      <c r="D82" s="39"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="20">
@@ -5275,7 +5315,7 @@
         <v>259</v>
       </c>
       <c r="C83" s="35"/>
-      <c r="D83" s="38"/>
+      <c r="D83" s="39"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="20">
@@ -5286,7 +5326,7 @@
         <v>106</v>
       </c>
       <c r="C84" s="35"/>
-      <c r="D84" s="38"/>
+      <c r="D84" s="39"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
@@ -5297,7 +5337,7 @@
         <v>260</v>
       </c>
       <c r="C85" s="35"/>
-      <c r="D85" s="38"/>
+      <c r="D85" s="39"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="20">
@@ -5319,6 +5359,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="D72:D85"/>
+    <mergeCell ref="D3:D71"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C75:C76"/>
     <mergeCell ref="E60:E68"/>
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="C58:C59"/>
@@ -5333,13 +5380,6 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C27:C37"/>
     <mergeCell ref="C39:C46"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="D72:D85"/>
-    <mergeCell ref="D3:D71"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C75:C76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>